<commit_message>
Added Xilinx docs, and changed the SAW/LNA to the *correct* part number
</commit_message>
<xml_diff>
--- a/v3-gps.xlsx
+++ b/v3-gps.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32" count="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30" count="30">
   <si>
     <t>0402 cap, X7R, 10%, Vw &gt;= 6V</t>
   </si>
@@ -109,12 +109,6 @@
   </si>
   <si>
     <t>MIC5319-1.8YD5</t>
-  </si>
-  <si>
-    <t>TOTAL</t>
-  </si>
-  <si>
-    <t>Boards to manufacture: </t>
   </si>
 </sst>
 </file>
@@ -264,8 +258,8 @@
   <dimension ref="A1:IV1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M72" sqref="M72"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H67" sqref="H67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -281,8 +275,7 @@
     <col min="9" max="11" style="2" width="9.142308"/>
     <col min="12" max="12" style="0" width="9.142308"/>
     <col min="13" max="13" style="2" width="20.71304" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" style="0" width="9.142308"/>
-    <col min="16" max="16384" style="0"/>
+    <col min="14" max="16384" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:256">
@@ -5160,7 +5153,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>ALM-GP002</t>
+          <t>ALM-GP003</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -5175,7 +5168,7 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>ALM-GP002-BLKG</t>
+          <t>ALM-GP003-BLKG</t>
         </is>
       </c>
       <c r="G67" t="s">
@@ -5183,7 +5176,7 @@
       </c>
       <c r="H67" s="10" t="inlineStr">
         <is>
-          <t>Mouser 630-ALM-GP002-BLKG</t>
+          <t>Mouser 630-ALM-GP003-BLKG</t>
         </is>
       </c>
       <c r="I67">
@@ -5597,8 +5590,10 @@
       </c>
     </row>
     <row r="73" spans="1:256">
-      <c r="L73" s="3" t="s">
-        <v>30</v>
+      <c r="L73" s="3" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
       </c>
       <c r="M73" s="15">
         <f>SUM(M2:M71)</f>
@@ -5606,8 +5601,10 @@
       </c>
     </row>
     <row r="75" spans="1:256">
-      <c r="A75" s="3" t="s">
-        <v>31</v>
+      <c r="A75" s="3" t="inlineStr">
+        <is>
+          <t>Boards to manufacture: </t>
+        </is>
       </c>
       <c r="D75" s="3">
         <v>3</v>

</xml_diff>

<commit_message>
Updated Schematic and BOM with problems, wrong values, etc.
</commit_message>
<xml_diff>
--- a/v3-gps.xlsx
+++ b/v3-gps.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30" count="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31" count="31">
   <si>
     <t>0402 cap, X7R, 10%, Vw &gt;= 6V</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>BP2G+</t>
+  </si>
+  <si>
+    <t>XC2C64A-5VQG44C</t>
   </si>
   <si>
     <t>MIC5319-1.8YD5</t>
@@ -258,7 +261,7 @@
   <dimension ref="A1:IV1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H67" sqref="H67"/>
     </sheetView>
   </sheetViews>
@@ -346,7 +349,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>C29, C30</t>
+          <t>C29,C30</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -380,7 +383,7 @@
         <v>0.0060000000000000001</v>
       </c>
       <c r="M2">
-        <f>IF($D$75*A2&lt;10,$D$75*A2*I2,IF($D$75*A2&lt;100,$D$75*A2*J2,$D$75*A2*K2))</f>
+        <f>IF($D$76*A2&lt;10,$D$76*A2*I2,IF($D$76*A2&lt;100,$D$76*A2*J2,$D$76*A2*K2))</f>
         <v>0.60000000000000009</v>
       </c>
     </row>
@@ -424,7 +427,7 @@
         <v>0.0060000000000000001</v>
       </c>
       <c r="M3">
-        <f>IF($D$75*A3&lt;10,$D$75*A3*I3,IF($D$75*A3&lt;100,$D$75*A3*J3,$D$75*A3*K3))</f>
+        <f>IF($D$76*A3&lt;10,$D$76*A3*I3,IF($D$76*A3&lt;100,$D$76*A3*J3,$D$76*A3*K3))</f>
         <v>0.30000000000000004</v>
       </c>
     </row>
@@ -468,7 +471,7 @@
         <v>0.0060000000000000001</v>
       </c>
       <c r="M4">
-        <f>IF($D$75*A4&lt;10,$D$75*A4*I4,IF($D$75*A4&lt;100,$D$75*A4*J4,$D$75*A4*K4))</f>
+        <f>IF($D$76*A4&lt;10,$D$76*A4*I4,IF($D$76*A4&lt;100,$D$76*A4*J4,$D$76*A4*K4))</f>
         <v>0.30000000000000004</v>
       </c>
     </row>
@@ -478,7 +481,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>C6, C8, C12, C14, C16, C17, C22, C57, C63, C80</t>
+          <t>C6,C8,C12,C14,C16,C17,C22,C57,C63,C80</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -512,7 +515,7 @@
         <v>0.0060000000000000001</v>
       </c>
       <c r="M5">
-        <f>IF($D$75*A5&lt;10,$D$75*A5*I5,IF($D$75*A5&lt;100,$D$75*A5*J5,$D$75*A5*K5))</f>
+        <f>IF($D$76*A5&lt;10,$D$76*A5*I5,IF($D$76*A5&lt;100,$D$76*A5*J5,$D$76*A5*K5))</f>
         <v>0.039</v>
       </c>
     </row>
@@ -556,7 +559,7 @@
         <v>0.0060000000000000001</v>
       </c>
       <c r="M6">
-        <f>IF($D$75*A6&lt;10,$D$75*A6*I6,IF($D$75*A6&lt;100,$D$75*A6*J6,$D$75*A6*K6))</f>
+        <f>IF($D$76*A6&lt;10,$D$76*A6*I6,IF($D$76*A6&lt;100,$D$76*A6*J6,$D$76*A6*K6))</f>
         <v>0.30000000000000004</v>
       </c>
     </row>
@@ -600,7 +603,7 @@
         <v>0.0060000000000000001</v>
       </c>
       <c r="M7">
-        <f>IF($D$75*A7&lt;10,$D$75*A7*I7,IF($D$75*A7&lt;100,$D$75*A7*J7,$D$75*A7*K7))</f>
+        <f>IF($D$76*A7&lt;10,$D$76*A7*I7,IF($D$76*A7&lt;100,$D$76*A7*J7,$D$76*A7*K7))</f>
         <v>0.30000000000000004</v>
       </c>
     </row>
@@ -644,7 +647,7 @@
         <v>0.033000000000000002</v>
       </c>
       <c r="M8">
-        <f>IF($D$75*A8&lt;10,$D$75*A8*I8,IF($D$75*A8&lt;100,$D$75*A8*J8,$D$75*A8*K8))</f>
+        <f>IF($D$76*A8&lt;10,$D$76*A8*I8,IF($D$76*A8&lt;100,$D$76*A8*J8,$D$76*A8*K8))</f>
         <v>0.60000000000000009</v>
       </c>
     </row>
@@ -654,7 +657,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>C2, C43, C60, C69, C77</t>
+          <t>C2,C43,C60,C69</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -688,7 +691,7 @@
         <v>0.0060000000000000001</v>
       </c>
       <c r="M9">
-        <f>IF($D$75*A9&lt;10,$D$75*A9*I9,IF($D$75*A9&lt;100,$D$75*A9*J9,$D$75*A9*K9))</f>
+        <f>IF($D$76*A9&lt;10,$D$76*A9*I9,IF($D$76*A9&lt;100,$D$76*A9*J9,$D$76*A9*K9))</f>
         <v>0.0195</v>
       </c>
     </row>
@@ -730,7 +733,7 @@
         <v>0.0060000000000000001</v>
       </c>
       <c r="M10">
-        <f>IF($D$75*A10&lt;10,$D$75*A10*I10,IF($D$75*A10&lt;100,$D$75*A10*J10,$D$75*A10*K10))</f>
+        <f>IF($D$76*A10&lt;10,$D$76*A10*I10,IF($D$76*A10&lt;100,$D$76*A10*J10,$D$76*A10*K10))</f>
         <v>0.30000000000000004</v>
       </c>
     </row>
@@ -740,7 +743,7 @@
       </c>
       <c r="B11" s="5" t="inlineStr">
         <is>
-          <t>C5, C7, C9, C10, C11, C13, C15, C18, C21, C23, C24, C27, C31, C34, C35, C37, C45, C46, C47, C48, C49, C50, C54, C55, C56, C61, C64, C70, C71, C72, C73, C74, C78, C82, C83, C84</t>
+          <t>C5,C7,C9,C10,C11,C13,C15,C18,C21,C23,C24,C27,C31,C34,C35,C37,C45,C46,C47,C48,C49,C50,C54,C55,C56,C61,C64,C70,C71,C72,C73,C74,C77,C78,C82,C83,C84</t>
         </is>
       </c>
       <c r="C11" s="6" t="inlineStr">
@@ -770,7 +773,7 @@
         <v>0.051999999999999998</v>
       </c>
       <c r="M11">
-        <f>IF($D$75*A11&lt;10,$D$75*A11*I11,IF($D$75*A11&lt;100,$D$75*A11*J11,$D$75*A11*K11))</f>
+        <f>IF($D$76*A11&lt;10,$D$76*A11*I11,IF($D$76*A11&lt;100,$D$76*A11*J11,$D$76*A11*K11))</f>
         <v>5.6159999999999997</v>
       </c>
     </row>
@@ -812,7 +815,7 @@
         <v>0.051999999999999998</v>
       </c>
       <c r="M12">
-        <f>IF($D$75*A12&lt;10,$D$75*A12*I12,IF($D$75*A12&lt;100,$D$75*A12*J12,$D$75*A12*K12))</f>
+        <f>IF($D$76*A12&lt;10,$D$76*A12*I12,IF($D$76*A12&lt;100,$D$76*A12*J12,$D$76*A12*K12))</f>
         <v>0.47999999999999998</v>
       </c>
     </row>
@@ -822,7 +825,7 @@
       </c>
       <c r="B13" s="5" t="inlineStr">
         <is>
-          <t>C19, C39, C40, C41, C42, C59, C67, C68, C75, C76, C79</t>
+          <t>C19,C39,C40,C41,C42,C59,C67,C68,C75,C79</t>
         </is>
       </c>
       <c r="C13" s="6" t="inlineStr">
@@ -852,7 +855,7 @@
         <v>0.051999999999999998</v>
       </c>
       <c r="M13">
-        <f>IF($D$75*A13&lt;10,$D$75*A13*I13,IF($D$75*A13&lt;100,$D$75*A13*J13,$D$75*A13*K13))</f>
+        <f>IF($D$76*A13&lt;10,$D$76*A13*I13,IF($D$76*A13&lt;100,$D$76*A13*J13,$D$76*A13*K13))</f>
         <v>3.6299999999999999</v>
       </c>
     </row>
@@ -894,7 +897,7 @@
         <v>0.051999999999999998</v>
       </c>
       <c r="M14">
-        <f>IF($D$75*A14&lt;10,$D$75*A14*I14,IF($D$75*A14&lt;100,$D$75*A14*J14,$D$75*A14*K14))</f>
+        <f>IF($D$76*A14&lt;10,$D$76*A14*I14,IF($D$76*A14&lt;100,$D$76*A14*J14,$D$76*A14*K14))</f>
         <v>0.47999999999999998</v>
       </c>
     </row>
@@ -904,7 +907,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>C20, C36, C51, C52, C53, C58</t>
+          <t>C20,C36,C51,C52,C53,C58,C76</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -938,7 +941,7 @@
         <v>0.039800000000000002</v>
       </c>
       <c r="M15">
-        <f>IF($D$75*A15&lt;10,$D$75*A15*I15,IF($D$75*A15&lt;100,$D$75*A15*J15,$D$75*A15*K15))</f>
+        <f>IF($D$76*A15&lt;10,$D$76*A15*I15,IF($D$76*A15&lt;100,$D$76*A15*J15,$D$76*A15*K15))</f>
         <v>15.66</v>
       </c>
     </row>
@@ -984,7 +987,7 @@
         <v>0.30299999999999999</v>
       </c>
       <c r="M16">
-        <f>IF($D$75*A16&lt;10,$D$75*A16*I16,IF($D$75*A16&lt;100,$D$75*A16*J16,$D$75*A16*K16))</f>
+        <f>IF($D$76*A16&lt;10,$D$76*A16*I16,IF($D$76*A16&lt;100,$D$76*A16*J16,$D$76*A16*K16))</f>
         <v>1.9500000000000002</v>
       </c>
     </row>
@@ -994,7 +997,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>C28, C32</t>
+          <t>C28,C32</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1030,7 +1033,7 @@
         <v>0.38400000000000001</v>
       </c>
       <c r="M17">
-        <f>IF($D$75*A17&lt;10,$D$75*A17*I17,IF($D$75*A17&lt;100,$D$75*A17*J17,$D$75*A17*K17))</f>
+        <f>IF($D$76*A17&lt;10,$D$76*A17*I17,IF($D$76*A17&lt;100,$D$76*A17*J17,$D$76*A17*K17))</f>
         <v>4.9799999999999995</v>
       </c>
     </row>
@@ -1078,7 +1081,7 @@
         <v>0.94999999999999996</v>
       </c>
       <c r="M18">
-        <f>IF($D$75*A18&lt;10,$D$75*A18*I18,IF($D$75*A18&lt;100,$D$75*A18*J18,$D$75*A18*K18))</f>
+        <f>IF($D$76*A18&lt;10,$D$76*A18*I18,IF($D$76*A18&lt;100,$D$76*A18*J18,$D$76*A18*K18))</f>
         <v>4.3200000000000003</v>
       </c>
     </row>
@@ -1126,7 +1129,7 @@
         <v>1.8400000000000001</v>
       </c>
       <c r="M19">
-        <f>IF($D$75*A19&lt;10,$D$75*A19*I19,IF($D$75*A19&lt;100,$D$75*A19*J19,$D$75*A19*K19))</f>
+        <f>IF($D$76*A19&lt;10,$D$76*A19*I19,IF($D$76*A19&lt;100,$D$76*A19*J19,$D$76*A19*K19))</f>
         <v>7.5600000000000005</v>
       </c>
     </row>
@@ -1393,7 +1396,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>D1, D2</t>
+          <t>D1,D2</t>
         </is>
       </c>
       <c r="C21" t="s">
@@ -1429,7 +1432,7 @@
         <v>0.217</v>
       </c>
       <c r="M21">
-        <f>IF($D$75*A21&lt;10,$D$75*A21*I21,IF($D$75*A21&lt;100,$D$75*A21*J21,$D$75*A21*K21))</f>
+        <f>IF($D$76*A21&lt;10,$D$76*A21*I21,IF($D$76*A21&lt;100,$D$76*A21*J21,$D$76*A21*K21))</f>
         <v>2.8199999999999998</v>
       </c>
     </row>
@@ -1735,7 +1738,7 @@
         <v>2.8900000000000001</v>
       </c>
       <c r="M23">
-        <f>IF($D$75*A23&lt;10,$D$75*A23*I23,IF($D$75*A23&lt;100,$D$75*A23*J23,$D$75*A23*K23))</f>
+        <f>IF($D$76*A23&lt;10,$D$76*A23*I23,IF($D$76*A23&lt;100,$D$76*A23*J23,$D$76*A23*K23))</f>
         <v>8.6699999999999999</v>
       </c>
     </row>
@@ -1781,7 +1784,7 @@
         <v>3.3300000000000001</v>
       </c>
       <c r="M24">
-        <f>IF($D$75*A24&lt;10,$D$75*A24*I24,IF($D$75*A24&lt;100,$D$75*A24*J24,$D$75*A24*K24))</f>
+        <f>IF($D$76*A24&lt;10,$D$76*A24*I24,IF($D$76*A24&lt;100,$D$76*A24*J24,$D$76*A24*K24))</f>
         <v>15.27</v>
       </c>
     </row>
@@ -1825,7 +1828,7 @@
         <v>1.145</v>
       </c>
       <c r="M25">
-        <f>IF($D$75*A25&lt;10,$D$75*A25*I25,IF($D$75*A25&lt;100,$D$75*A25*J25,$D$75*A25*K25))</f>
+        <f>IF($D$76*A25&lt;10,$D$76*A25*I25,IF($D$76*A25&lt;100,$D$76*A25*J25,$D$76*A25*K25))</f>
         <v>4.4100000000000001</v>
       </c>
     </row>
@@ -1869,7 +1872,7 @@
         <v>0.91200000000000003</v>
       </c>
       <c r="M26">
-        <f>IF($D$75*A26&lt;10,$D$75*A26*I26,IF($D$75*A26&lt;100,$D$75*A26*J26,$D$75*A26*K26))</f>
+        <f>IF($D$76*A26&lt;10,$D$76*A26*I26,IF($D$76*A26&lt;100,$D$76*A26*J26,$D$76*A26*K26))</f>
         <v>3.5999999999999996</v>
       </c>
     </row>
@@ -1913,7 +1916,7 @@
         <v>1.46</v>
       </c>
       <c r="M27">
-        <f>IF($D$75*A27&lt;10,$D$75*A27*I27,IF($D$75*A27&lt;100,$D$75*A27*J27,$D$75*A27*K27))</f>
+        <f>IF($D$76*A27&lt;10,$D$76*A27*I27,IF($D$76*A27&lt;100,$D$76*A27*J27,$D$76*A27*K27))</f>
         <v>5.6399999999999997</v>
       </c>
     </row>
@@ -1957,7 +1960,7 @@
         <v>0.16900000000000001</v>
       </c>
       <c r="M28">
-        <f>IF($D$75*A28&lt;10,$D$75*A28*I28,IF($D$75*A28&lt;100,$D$75*A28*J28,$D$75*A28*K28))</f>
+        <f>IF($D$76*A28&lt;10,$D$76*A28*I28,IF($D$76*A28&lt;100,$D$76*A28*J28,$D$76*A28*K28))</f>
         <v>0.78000000000000003</v>
       </c>
     </row>
@@ -2224,7 +2227,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>L1, L4</t>
+          <t>L1,L4</t>
         </is>
       </c>
       <c r="C30" t="s">
@@ -2258,7 +2261,7 @@
         <v>0.33600000000000002</v>
       </c>
       <c r="M30">
-        <f>IF($D$75*A30&lt;10,$D$75*A30*I30,IF($D$75*A30&lt;100,$D$75*A30*J30,$D$75*A30*K30))</f>
+        <f>IF($D$76*A30&lt;10,$D$76*A30*I30,IF($D$76*A30&lt;100,$D$76*A30*J30,$D$76*A30*K30))</f>
         <v>3</v>
       </c>
     </row>
@@ -2302,7 +2305,7 @@
         <v>0.124</v>
       </c>
       <c r="M31">
-        <f>IF($D$75*A31&lt;10,$D$75*A31*I31,IF($D$75*A31&lt;100,$D$75*A31*J31,$D$75*A31*K31))</f>
+        <f>IF($D$76*A31&lt;10,$D$76*A31*I31,IF($D$76*A31&lt;100,$D$76*A31*J31,$D$76*A31*K31))</f>
         <v>0.75</v>
       </c>
     </row>
@@ -2342,7 +2345,7 @@
         <v>10</v>
       </c>
       <c r="M32">
-        <f>IF($D$75*A32&lt;10,$D$75*A32*I32,IF($D$75*A32&lt;100,$D$75*A32*J32,$D$75*A32*K32))</f>
+        <f>IF($D$76*A32&lt;10,$D$76*A32*I32,IF($D$76*A32&lt;100,$D$76*A32*J32,$D$76*A32*K32))</f>
         <v>0</v>
       </c>
     </row>
@@ -2386,7 +2389,7 @@
         <v>0.065000000000000002</v>
       </c>
       <c r="M33">
-        <f>IF($D$75*A33&lt;10,$D$75*A33*I33,IF($D$75*A33&lt;100,$D$75*A33*J33,$D$75*A33*K33))</f>
+        <f>IF($D$76*A33&lt;10,$D$76*A33*I33,IF($D$76*A33&lt;100,$D$76*A33*J33,$D$76*A33*K33))</f>
         <v>0.23999999999999999</v>
       </c>
     </row>
@@ -2430,7 +2433,7 @@
         <v>0.20599999999999999</v>
       </c>
       <c r="M34">
-        <f>IF($D$75*A34&lt;10,$D$75*A34*I34,IF($D$75*A34&lt;100,$D$75*A34*J34,$D$75*A34*K34))</f>
+        <f>IF($D$76*A34&lt;10,$D$76*A34*I34,IF($D$76*A34&lt;100,$D$76*A34*J34,$D$76*A34*K34))</f>
         <v>0.95999999999999996</v>
       </c>
     </row>
@@ -2733,7 +2736,7 @@
         <v>0.085000000000000006</v>
       </c>
       <c r="M36">
-        <f>IF($D$75*A36&lt;10,$D$75*A36*I36,IF($D$75*A36&lt;100,$D$75*A36*J36,$D$75*A36*K36))</f>
+        <f>IF($D$76*A36&lt;10,$D$76*A36*I36,IF($D$76*A36&lt;100,$D$76*A36*J36,$D$76*A36*K36))</f>
         <v>0.47999999999999998</v>
       </c>
     </row>
@@ -2743,7 +2746,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>LED2, LED4, LED5, LED6, LED7</t>
+          <t>LED2,LED4,LED5,LED6,LED7</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -2779,7 +2782,7 @@
         <v>0.085000000000000006</v>
       </c>
       <c r="M37">
-        <f>IF($D$75*A37&lt;10,$D$75*A37*I37,IF($D$75*A37&lt;100,$D$75*A37*J37,$D$75*A37*K37))</f>
+        <f>IF($D$76*A37&lt;10,$D$76*A37*I37,IF($D$76*A37&lt;100,$D$76*A37*J37,$D$76*A37*K37))</f>
         <v>1.7550000000000001</v>
       </c>
     </row>
@@ -2823,7 +2826,7 @@
         <v>1.22</v>
       </c>
       <c r="M38">
-        <f>IF($D$75*A38&lt;10,$D$75*A38*I38,IF($D$75*A38&lt;100,$D$75*A38*J38,$D$75*A38*K38))</f>
+        <f>IF($D$76*A38&lt;10,$D$76*A38*I38,IF($D$76*A38&lt;100,$D$76*A38*J38,$D$76*A38*K38))</f>
         <v>6.6000000000000005</v>
       </c>
     </row>
@@ -3124,7 +3127,7 @@
         <v>0.20799999999999999</v>
       </c>
       <c r="M40">
-        <f>IF($D$75*A40&lt;10,$D$75*A40*I40,IF($D$75*A40&lt;100,$D$75*A40*J40,$D$75*A40*K40))</f>
+        <f>IF($D$76*A40&lt;10,$D$76*A40*I40,IF($D$76*A40&lt;100,$D$76*A40*J40,$D$76*A40*K40))</f>
         <v>1.3500000000000001</v>
       </c>
     </row>
@@ -3423,7 +3426,7 @@
         <v>0.014999999999999999</v>
       </c>
       <c r="M42">
-        <f>IF($D$75*A42&lt;10,$D$75*A42*I42,IF($D$75*A42&lt;100,$D$75*A42*J42,$D$75*A42*K42))</f>
+        <f>IF($D$76*A42&lt;10,$D$76*A42*I42,IF($D$76*A42&lt;100,$D$76*A42*J42,$D$76*A42*K42))</f>
         <v>0.30000000000000004</v>
       </c>
     </row>
@@ -3433,7 +3436,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>R10, R11</t>
+          <t>R10,R11</t>
         </is>
       </c>
       <c r="C43">
@@ -3465,7 +3468,7 @@
         <v>0.014999999999999999</v>
       </c>
       <c r="M43">
-        <f>IF($D$75*A43&lt;10,$D$75*A43*I43,IF($D$75*A43&lt;100,$D$75*A43*J43,$D$75*A43*K43))</f>
+        <f>IF($D$76*A43&lt;10,$D$76*A43*I43,IF($D$76*A43&lt;100,$D$76*A43*J43,$D$76*A43*K43))</f>
         <v>0.60000000000000009</v>
       </c>
     </row>
@@ -3475,7 +3478,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>R4, R6, R17, R23, R42, R43</t>
+          <t>R4,R6,R17,R23,R24,R42,R43</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -3509,7 +3512,7 @@
         <v>0.014999999999999999</v>
       </c>
       <c r="M44">
-        <f>IF($D$75*A44&lt;10,$D$75*A44*I44,IF($D$75*A44&lt;100,$D$75*A44*J44,$D$75*A44*K44))</f>
+        <f>IF($D$76*A44&lt;10,$D$76*A44*I44,IF($D$76*A44&lt;100,$D$76*A44*J44,$D$76*A44*K44))</f>
         <v>0.34199999999999997</v>
       </c>
     </row>
@@ -3553,7 +3556,7 @@
         <v>0.014999999999999999</v>
       </c>
       <c r="M45">
-        <f>IF($D$75*A45&lt;10,$D$75*A45*I45,IF($D$75*A45&lt;100,$D$75*A45*J45,$D$75*A45*K45))</f>
+        <f>IF($D$76*A45&lt;10,$D$76*A45*I45,IF($D$76*A45&lt;100,$D$76*A45*J45,$D$76*A45*K45))</f>
         <v>0.30000000000000004</v>
       </c>
     </row>
@@ -3563,7 +3566,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>R1, R14, R16, R20, R38, R39, R40</t>
+          <t>R1,R14,R16,R20,R38,R39,R40</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -3597,7 +3600,7 @@
         <v>0.014999999999999999</v>
       </c>
       <c r="M46">
-        <f>IF($D$75*A46&lt;10,$D$75*A46*I46,IF($D$75*A46&lt;100,$D$75*A46*J46,$D$75*A46*K46))</f>
+        <f>IF($D$76*A46&lt;10,$D$76*A46*I46,IF($D$76*A46&lt;100,$D$76*A46*J46,$D$76*A46*K46))</f>
         <v>0.39899999999999997</v>
       </c>
     </row>
@@ -3641,7 +3644,7 @@
         <v>0.014999999999999999</v>
       </c>
       <c r="M47">
-        <f>IF($D$75*A47&lt;10,$D$75*A47*I47,IF($D$75*A47&lt;100,$D$75*A47*J47,$D$75*A47*K47))</f>
+        <f>IF($D$76*A47&lt;10,$D$76*A47*I47,IF($D$76*A47&lt;100,$D$76*A47*J47,$D$76*A47*K47))</f>
         <v>0.30000000000000004</v>
       </c>
     </row>
@@ -3685,7 +3688,7 @@
         <v>0.014999999999999999</v>
       </c>
       <c r="M48">
-        <f>IF($D$75*A48&lt;10,$D$75*A48*I48,IF($D$75*A48&lt;100,$D$75*A48*J48,$D$75*A48*K48))</f>
+        <f>IF($D$76*A48&lt;10,$D$76*A48*I48,IF($D$76*A48&lt;100,$D$76*A48*J48,$D$76*A48*K48))</f>
         <v>0.30000000000000004</v>
       </c>
     </row>
@@ -3695,7 +3698,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>R5, R8, R9, R12, R18, R19, R21, R22, R24, R26, R27</t>
+          <t>R5,R8,R9,R12,R18,R19,R22,R26,R27</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -3729,7 +3732,7 @@
         <v>0.014999999999999999</v>
       </c>
       <c r="M49">
-        <f>IF($D$75*A49&lt;10,$D$75*A49*I49,IF($D$75*A49&lt;100,$D$75*A49*J49,$D$75*A49*K49))</f>
+        <f>IF($D$76*A49&lt;10,$D$76*A49*I49,IF($D$76*A49&lt;100,$D$76*A49*J49,$D$76*A49*K49))</f>
         <v>0.627</v>
       </c>
     </row>
@@ -3773,7 +3776,7 @@
         <v>0.014999999999999999</v>
       </c>
       <c r="M50">
-        <f>IF($D$75*A50&lt;10,$D$75*A50*I50,IF($D$75*A50&lt;100,$D$75*A50*J50,$D$75*A50*K50))</f>
+        <f>IF($D$76*A50&lt;10,$D$76*A50*I50,IF($D$76*A50&lt;100,$D$76*A50*J50,$D$76*A50*K50))</f>
         <v>0.30000000000000004</v>
       </c>
     </row>
@@ -3783,12 +3786,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>R7</t>
+          <t>R21</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>61.9k</t>
+          <t>33k</t>
         </is>
       </c>
       <c r="D51" t="s">
@@ -3799,12 +3802,12 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>ERJ-2RKF6192X</t>
+          <t>ERJ-2RKF3302X</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>P61.9KLCT-ND</t>
+          <t>P33.0KLCT-ND</t>
         </is>
       </c>
       <c r="I51">
@@ -3817,308 +3820,310 @@
         <v>0.014999999999999999</v>
       </c>
       <c r="M51">
-        <f>IF($D$75*A51&lt;10,$D$75*A51*I51,IF($D$75*A51&lt;100,$D$75*A51*J51,$D$75*A51*K51))</f>
+        <f>IF($D$76*A51&lt;10,$D$76*A51*I51,IF($D$76*A51&lt;100,$D$76*A51*J51,$D$76*A51*K51))</f>
         <v>0.30000000000000004</v>
       </c>
     </row>
     <row r="52" spans="1:256">
-      <c r="A52" s="7"/>
-      <c r="B52" s="7"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="7"/>
-      <c r="E52" s="7"/>
-      <c r="F52" s="7"/>
-      <c r="G52" s="7"/>
-      <c r="H52" s="7"/>
-      <c r="I52" s="9"/>
-      <c r="J52" s="9"/>
-      <c r="K52" s="9"/>
-      <c r="L52" s="7"/>
-      <c r="M52" s="9"/>
-      <c r="N52" s="7"/>
-      <c r="O52" s="7"/>
-      <c r="P52" s="7"/>
-      <c r="Q52" s="7"/>
-      <c r="R52" s="7"/>
-      <c r="S52" s="7"/>
-      <c r="T52" s="7"/>
-      <c r="U52" s="7"/>
-      <c r="V52" s="7"/>
-      <c r="W52" s="7"/>
-      <c r="X52" s="7"/>
-      <c r="Y52" s="7"/>
-      <c r="Z52" s="7"/>
-      <c r="AA52" s="7"/>
-      <c r="AB52" s="7"/>
-      <c r="AC52" s="7"/>
-      <c r="AD52" s="7"/>
-      <c r="AE52" s="7"/>
-      <c r="AF52" s="7"/>
-      <c r="AG52" s="7"/>
-      <c r="AH52" s="7"/>
-      <c r="AI52" s="7"/>
-      <c r="AJ52" s="7"/>
-      <c r="AK52" s="7"/>
-      <c r="AL52" s="7"/>
-      <c r="AM52" s="7"/>
-      <c r="AN52" s="7"/>
-      <c r="AO52" s="7"/>
-      <c r="AP52" s="7"/>
-      <c r="AQ52" s="7"/>
-      <c r="AR52" s="7"/>
-      <c r="AS52" s="7"/>
-      <c r="AT52" s="7"/>
-      <c r="AU52" s="7"/>
-      <c r="AV52" s="7"/>
-      <c r="AW52" s="7"/>
-      <c r="AX52" s="7"/>
-      <c r="AY52" s="7"/>
-      <c r="AZ52" s="7"/>
-      <c r="BA52" s="7"/>
-      <c r="BB52" s="7"/>
-      <c r="BC52" s="7"/>
-      <c r="BD52" s="7"/>
-      <c r="BE52" s="7"/>
-      <c r="BF52" s="7"/>
-      <c r="BG52" s="7"/>
-      <c r="BH52" s="7"/>
-      <c r="BI52" s="7"/>
-      <c r="BJ52" s="7"/>
-      <c r="BK52" s="7"/>
-      <c r="BL52" s="7"/>
-      <c r="BM52" s="7"/>
-      <c r="BN52" s="7"/>
-      <c r="BO52" s="7"/>
-      <c r="BP52" s="7"/>
-      <c r="BQ52" s="7"/>
-      <c r="BR52" s="7"/>
-      <c r="BS52" s="7"/>
-      <c r="BT52" s="7"/>
-      <c r="BU52" s="7"/>
-      <c r="BV52" s="7"/>
-      <c r="BW52" s="7"/>
-      <c r="BX52" s="7"/>
-      <c r="BY52" s="7"/>
-      <c r="BZ52" s="7"/>
-      <c r="CA52" s="7"/>
-      <c r="CB52" s="7"/>
-      <c r="CC52" s="7"/>
-      <c r="CD52" s="7"/>
-      <c r="CE52" s="7"/>
-      <c r="CF52" s="7"/>
-      <c r="CG52" s="7"/>
-      <c r="CH52" s="7"/>
-      <c r="CI52" s="7"/>
-      <c r="CJ52" s="7"/>
-      <c r="CK52" s="7"/>
-      <c r="CL52" s="7"/>
-      <c r="CM52" s="7"/>
-      <c r="CN52" s="7"/>
-      <c r="CO52" s="7"/>
-      <c r="CP52" s="7"/>
-      <c r="CQ52" s="7"/>
-      <c r="CR52" s="7"/>
-      <c r="CS52" s="7"/>
-      <c r="CT52" s="7"/>
-      <c r="CU52" s="7"/>
-      <c r="CV52" s="7"/>
-      <c r="CW52" s="7"/>
-      <c r="CX52" s="7"/>
-      <c r="CY52" s="7"/>
-      <c r="CZ52" s="7"/>
-      <c r="DA52" s="7"/>
-      <c r="DB52" s="7"/>
-      <c r="DC52" s="7"/>
-      <c r="DD52" s="7"/>
-      <c r="DE52" s="7"/>
-      <c r="DF52" s="7"/>
-      <c r="DG52" s="7"/>
-      <c r="DH52" s="7"/>
-      <c r="DI52" s="7"/>
-      <c r="DJ52" s="7"/>
-      <c r="DK52" s="7"/>
-      <c r="DL52" s="7"/>
-      <c r="DM52" s="7"/>
-      <c r="DN52" s="7"/>
-      <c r="DO52" s="7"/>
-      <c r="DP52" s="7"/>
-      <c r="DQ52" s="7"/>
-      <c r="DR52" s="7"/>
-      <c r="DS52" s="7"/>
-      <c r="DT52" s="7"/>
-      <c r="DU52" s="7"/>
-      <c r="DV52" s="7"/>
-      <c r="DW52" s="7"/>
-      <c r="DX52" s="7"/>
-      <c r="DY52" s="7"/>
-      <c r="DZ52" s="7"/>
-      <c r="EA52" s="7"/>
-      <c r="EB52" s="7"/>
-      <c r="EC52" s="7"/>
-      <c r="ED52" s="7"/>
-      <c r="EE52" s="7"/>
-      <c r="EF52" s="7"/>
-      <c r="EG52" s="7"/>
-      <c r="EH52" s="7"/>
-      <c r="EI52" s="7"/>
-      <c r="EJ52" s="7"/>
-      <c r="EK52" s="7"/>
-      <c r="EL52" s="7"/>
-      <c r="EM52" s="7"/>
-      <c r="EN52" s="7"/>
-      <c r="EO52" s="7"/>
-      <c r="EP52" s="7"/>
-      <c r="EQ52" s="7"/>
-      <c r="ER52" s="7"/>
-      <c r="ES52" s="7"/>
-      <c r="ET52" s="7"/>
-      <c r="EU52" s="7"/>
-      <c r="EV52" s="7"/>
-      <c r="EW52" s="7"/>
-      <c r="EX52" s="7"/>
-      <c r="EY52" s="7"/>
-      <c r="EZ52" s="7"/>
-      <c r="FA52" s="7"/>
-      <c r="FB52" s="7"/>
-      <c r="FC52" s="7"/>
-      <c r="FD52" s="7"/>
-      <c r="FE52" s="7"/>
-      <c r="FF52" s="7"/>
-      <c r="FG52" s="7"/>
-      <c r="FH52" s="7"/>
-      <c r="FI52" s="7"/>
-      <c r="FJ52" s="7"/>
-      <c r="FK52" s="7"/>
-      <c r="FL52" s="7"/>
-      <c r="FM52" s="7"/>
-      <c r="FN52" s="7"/>
-      <c r="FO52" s="7"/>
-      <c r="FP52" s="7"/>
-      <c r="FQ52" s="7"/>
-      <c r="FR52" s="7"/>
-      <c r="FS52" s="7"/>
-      <c r="FT52" s="7"/>
-      <c r="FU52" s="7"/>
-      <c r="FV52" s="7"/>
-      <c r="FW52" s="7"/>
-      <c r="FX52" s="7"/>
-      <c r="FY52" s="7"/>
-      <c r="FZ52" s="7"/>
-      <c r="GA52" s="7"/>
-      <c r="GB52" s="7"/>
-      <c r="GC52" s="7"/>
-      <c r="GD52" s="7"/>
-      <c r="GE52" s="7"/>
-      <c r="GF52" s="7"/>
-      <c r="GG52" s="7"/>
-      <c r="GH52" s="7"/>
-      <c r="GI52" s="7"/>
-      <c r="GJ52" s="7"/>
-      <c r="GK52" s="7"/>
-      <c r="GL52" s="7"/>
-      <c r="GM52" s="7"/>
-      <c r="GN52" s="7"/>
-      <c r="GO52" s="7"/>
-      <c r="GP52" s="7"/>
-      <c r="GQ52" s="7"/>
-      <c r="GR52" s="7"/>
-      <c r="GS52" s="7"/>
-      <c r="GT52" s="7"/>
-      <c r="GU52" s="7"/>
-      <c r="GV52" s="7"/>
-      <c r="GW52" s="7"/>
-      <c r="GX52" s="7"/>
-      <c r="GY52" s="7"/>
-      <c r="GZ52" s="7"/>
-      <c r="HA52" s="7"/>
-      <c r="HB52" s="7"/>
-      <c r="HC52" s="7"/>
-      <c r="HD52" s="7"/>
-      <c r="HE52" s="7"/>
-      <c r="HF52" s="7"/>
-      <c r="HG52" s="7"/>
-      <c r="HH52" s="7"/>
-      <c r="HI52" s="7"/>
-      <c r="HJ52" s="7"/>
-      <c r="HK52" s="7"/>
-      <c r="HL52" s="7"/>
-      <c r="HM52" s="7"/>
-      <c r="HN52" s="7"/>
-      <c r="HO52" s="7"/>
-      <c r="HP52" s="7"/>
-      <c r="HQ52" s="7"/>
-      <c r="HR52" s="7"/>
-      <c r="HS52" s="7"/>
-      <c r="HT52" s="7"/>
-      <c r="HU52" s="7"/>
-      <c r="HV52" s="7"/>
-      <c r="HW52" s="7"/>
-      <c r="HX52" s="7"/>
-      <c r="HY52" s="7"/>
-      <c r="HZ52" s="7"/>
-      <c r="IA52" s="7"/>
-      <c r="IB52" s="7"/>
-      <c r="IC52" s="7"/>
-      <c r="ID52" s="7"/>
-      <c r="IE52" s="7"/>
-      <c r="IF52" s="7"/>
-      <c r="IG52" s="7"/>
-      <c r="IH52" s="7"/>
-      <c r="II52" s="7"/>
-      <c r="IJ52" s="7"/>
-      <c r="IK52" s="7"/>
-      <c r="IL52" s="7"/>
-      <c r="IM52" s="7"/>
-      <c r="IN52" s="7"/>
-      <c r="IO52" s="7"/>
-      <c r="IP52" s="7"/>
-      <c r="IQ52" s="7"/>
-      <c r="IR52" s="7"/>
-      <c r="IS52" s="7"/>
-      <c r="IT52" s="7"/>
-      <c r="IU52" s="7"/>
+      <c r="A52">
+        <v>1</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>R7</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>61.9k</t>
+        </is>
+      </c>
+      <c r="D52" t="s">
+        <v>18</v>
+      </c>
+      <c r="E52" t="s">
+        <v>14</v>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>ERJ-2RKF6192X</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>P61.9KLCT-ND</t>
+        </is>
+      </c>
+      <c r="I52">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="J52">
+        <v>0.019</v>
+      </c>
+      <c r="K52">
+        <v>0.014999999999999999</v>
+      </c>
+      <c r="M52">
+        <f>IF($D$76*A52&lt;10,$D$76*A52*I52,IF($D$76*A52&lt;100,$D$76*A52*J52,$D$76*A52*K52))</f>
+        <v>0.30000000000000004</v>
+      </c>
     </row>
     <row r="53" spans="1:256">
-      <c r="A53">
-        <v>1</v>
-      </c>
-      <c r="B53" t="s">
-        <v>19</v>
-      </c>
-      <c r="C53" t="s">
-        <v>20</v>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>RF shield with removable cover</t>
-        </is>
-      </c>
-      <c r="E53" t="s">
-        <v>21</v>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>BMI-S-202-F</t>
-        </is>
-      </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>903-1051-1-ND</t>
-        </is>
-      </c>
-      <c r="I53">
-        <v>1.79</v>
-      </c>
-      <c r="J53">
-        <v>1.5800000000000001</v>
-      </c>
-      <c r="K53">
-        <v>1.25</v>
-      </c>
-      <c r="M53">
-        <f>IF($D$75*A53&lt;10,$D$75*A53*I53,IF($D$75*A53&lt;100,$D$75*A53*J53,$D$75*A53*K53))</f>
-        <v>5.3700000000000001</v>
-      </c>
+      <c r="A53" s="7"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7"/>
+      <c r="H53" s="7"/>
+      <c r="I53" s="9"/>
+      <c r="J53" s="9"/>
+      <c r="K53" s="9"/>
+      <c r="L53" s="7"/>
+      <c r="M53" s="9"/>
+      <c r="N53" s="7"/>
+      <c r="O53" s="7"/>
+      <c r="P53" s="7"/>
+      <c r="Q53" s="7"/>
+      <c r="R53" s="7"/>
+      <c r="S53" s="7"/>
+      <c r="T53" s="7"/>
+      <c r="U53" s="7"/>
+      <c r="V53" s="7"/>
+      <c r="W53" s="7"/>
+      <c r="X53" s="7"/>
+      <c r="Y53" s="7"/>
+      <c r="Z53" s="7"/>
+      <c r="AA53" s="7"/>
+      <c r="AB53" s="7"/>
+      <c r="AC53" s="7"/>
+      <c r="AD53" s="7"/>
+      <c r="AE53" s="7"/>
+      <c r="AF53" s="7"/>
+      <c r="AG53" s="7"/>
+      <c r="AH53" s="7"/>
+      <c r="AI53" s="7"/>
+      <c r="AJ53" s="7"/>
+      <c r="AK53" s="7"/>
+      <c r="AL53" s="7"/>
+      <c r="AM53" s="7"/>
+      <c r="AN53" s="7"/>
+      <c r="AO53" s="7"/>
+      <c r="AP53" s="7"/>
+      <c r="AQ53" s="7"/>
+      <c r="AR53" s="7"/>
+      <c r="AS53" s="7"/>
+      <c r="AT53" s="7"/>
+      <c r="AU53" s="7"/>
+      <c r="AV53" s="7"/>
+      <c r="AW53" s="7"/>
+      <c r="AX53" s="7"/>
+      <c r="AY53" s="7"/>
+      <c r="AZ53" s="7"/>
+      <c r="BA53" s="7"/>
+      <c r="BB53" s="7"/>
+      <c r="BC53" s="7"/>
+      <c r="BD53" s="7"/>
+      <c r="BE53" s="7"/>
+      <c r="BF53" s="7"/>
+      <c r="BG53" s="7"/>
+      <c r="BH53" s="7"/>
+      <c r="BI53" s="7"/>
+      <c r="BJ53" s="7"/>
+      <c r="BK53" s="7"/>
+      <c r="BL53" s="7"/>
+      <c r="BM53" s="7"/>
+      <c r="BN53" s="7"/>
+      <c r="BO53" s="7"/>
+      <c r="BP53" s="7"/>
+      <c r="BQ53" s="7"/>
+      <c r="BR53" s="7"/>
+      <c r="BS53" s="7"/>
+      <c r="BT53" s="7"/>
+      <c r="BU53" s="7"/>
+      <c r="BV53" s="7"/>
+      <c r="BW53" s="7"/>
+      <c r="BX53" s="7"/>
+      <c r="BY53" s="7"/>
+      <c r="BZ53" s="7"/>
+      <c r="CA53" s="7"/>
+      <c r="CB53" s="7"/>
+      <c r="CC53" s="7"/>
+      <c r="CD53" s="7"/>
+      <c r="CE53" s="7"/>
+      <c r="CF53" s="7"/>
+      <c r="CG53" s="7"/>
+      <c r="CH53" s="7"/>
+      <c r="CI53" s="7"/>
+      <c r="CJ53" s="7"/>
+      <c r="CK53" s="7"/>
+      <c r="CL53" s="7"/>
+      <c r="CM53" s="7"/>
+      <c r="CN53" s="7"/>
+      <c r="CO53" s="7"/>
+      <c r="CP53" s="7"/>
+      <c r="CQ53" s="7"/>
+      <c r="CR53" s="7"/>
+      <c r="CS53" s="7"/>
+      <c r="CT53" s="7"/>
+      <c r="CU53" s="7"/>
+      <c r="CV53" s="7"/>
+      <c r="CW53" s="7"/>
+      <c r="CX53" s="7"/>
+      <c r="CY53" s="7"/>
+      <c r="CZ53" s="7"/>
+      <c r="DA53" s="7"/>
+      <c r="DB53" s="7"/>
+      <c r="DC53" s="7"/>
+      <c r="DD53" s="7"/>
+      <c r="DE53" s="7"/>
+      <c r="DF53" s="7"/>
+      <c r="DG53" s="7"/>
+      <c r="DH53" s="7"/>
+      <c r="DI53" s="7"/>
+      <c r="DJ53" s="7"/>
+      <c r="DK53" s="7"/>
+      <c r="DL53" s="7"/>
+      <c r="DM53" s="7"/>
+      <c r="DN53" s="7"/>
+      <c r="DO53" s="7"/>
+      <c r="DP53" s="7"/>
+      <c r="DQ53" s="7"/>
+      <c r="DR53" s="7"/>
+      <c r="DS53" s="7"/>
+      <c r="DT53" s="7"/>
+      <c r="DU53" s="7"/>
+      <c r="DV53" s="7"/>
+      <c r="DW53" s="7"/>
+      <c r="DX53" s="7"/>
+      <c r="DY53" s="7"/>
+      <c r="DZ53" s="7"/>
+      <c r="EA53" s="7"/>
+      <c r="EB53" s="7"/>
+      <c r="EC53" s="7"/>
+      <c r="ED53" s="7"/>
+      <c r="EE53" s="7"/>
+      <c r="EF53" s="7"/>
+      <c r="EG53" s="7"/>
+      <c r="EH53" s="7"/>
+      <c r="EI53" s="7"/>
+      <c r="EJ53" s="7"/>
+      <c r="EK53" s="7"/>
+      <c r="EL53" s="7"/>
+      <c r="EM53" s="7"/>
+      <c r="EN53" s="7"/>
+      <c r="EO53" s="7"/>
+      <c r="EP53" s="7"/>
+      <c r="EQ53" s="7"/>
+      <c r="ER53" s="7"/>
+      <c r="ES53" s="7"/>
+      <c r="ET53" s="7"/>
+      <c r="EU53" s="7"/>
+      <c r="EV53" s="7"/>
+      <c r="EW53" s="7"/>
+      <c r="EX53" s="7"/>
+      <c r="EY53" s="7"/>
+      <c r="EZ53" s="7"/>
+      <c r="FA53" s="7"/>
+      <c r="FB53" s="7"/>
+      <c r="FC53" s="7"/>
+      <c r="FD53" s="7"/>
+      <c r="FE53" s="7"/>
+      <c r="FF53" s="7"/>
+      <c r="FG53" s="7"/>
+      <c r="FH53" s="7"/>
+      <c r="FI53" s="7"/>
+      <c r="FJ53" s="7"/>
+      <c r="FK53" s="7"/>
+      <c r="FL53" s="7"/>
+      <c r="FM53" s="7"/>
+      <c r="FN53" s="7"/>
+      <c r="FO53" s="7"/>
+      <c r="FP53" s="7"/>
+      <c r="FQ53" s="7"/>
+      <c r="FR53" s="7"/>
+      <c r="FS53" s="7"/>
+      <c r="FT53" s="7"/>
+      <c r="FU53" s="7"/>
+      <c r="FV53" s="7"/>
+      <c r="FW53" s="7"/>
+      <c r="FX53" s="7"/>
+      <c r="FY53" s="7"/>
+      <c r="FZ53" s="7"/>
+      <c r="GA53" s="7"/>
+      <c r="GB53" s="7"/>
+      <c r="GC53" s="7"/>
+      <c r="GD53" s="7"/>
+      <c r="GE53" s="7"/>
+      <c r="GF53" s="7"/>
+      <c r="GG53" s="7"/>
+      <c r="GH53" s="7"/>
+      <c r="GI53" s="7"/>
+      <c r="GJ53" s="7"/>
+      <c r="GK53" s="7"/>
+      <c r="GL53" s="7"/>
+      <c r="GM53" s="7"/>
+      <c r="GN53" s="7"/>
+      <c r="GO53" s="7"/>
+      <c r="GP53" s="7"/>
+      <c r="GQ53" s="7"/>
+      <c r="GR53" s="7"/>
+      <c r="GS53" s="7"/>
+      <c r="GT53" s="7"/>
+      <c r="GU53" s="7"/>
+      <c r="GV53" s="7"/>
+      <c r="GW53" s="7"/>
+      <c r="GX53" s="7"/>
+      <c r="GY53" s="7"/>
+      <c r="GZ53" s="7"/>
+      <c r="HA53" s="7"/>
+      <c r="HB53" s="7"/>
+      <c r="HC53" s="7"/>
+      <c r="HD53" s="7"/>
+      <c r="HE53" s="7"/>
+      <c r="HF53" s="7"/>
+      <c r="HG53" s="7"/>
+      <c r="HH53" s="7"/>
+      <c r="HI53" s="7"/>
+      <c r="HJ53" s="7"/>
+      <c r="HK53" s="7"/>
+      <c r="HL53" s="7"/>
+      <c r="HM53" s="7"/>
+      <c r="HN53" s="7"/>
+      <c r="HO53" s="7"/>
+      <c r="HP53" s="7"/>
+      <c r="HQ53" s="7"/>
+      <c r="HR53" s="7"/>
+      <c r="HS53" s="7"/>
+      <c r="HT53" s="7"/>
+      <c r="HU53" s="7"/>
+      <c r="HV53" s="7"/>
+      <c r="HW53" s="7"/>
+      <c r="HX53" s="7"/>
+      <c r="HY53" s="7"/>
+      <c r="HZ53" s="7"/>
+      <c r="IA53" s="7"/>
+      <c r="IB53" s="7"/>
+      <c r="IC53" s="7"/>
+      <c r="ID53" s="7"/>
+      <c r="IE53" s="7"/>
+      <c r="IF53" s="7"/>
+      <c r="IG53" s="7"/>
+      <c r="IH53" s="7"/>
+      <c r="II53" s="7"/>
+      <c r="IJ53" s="7"/>
+      <c r="IK53" s="7"/>
+      <c r="IL53" s="7"/>
+      <c r="IM53" s="7"/>
+      <c r="IN53" s="7"/>
+      <c r="IO53" s="7"/>
+      <c r="IP53" s="7"/>
+      <c r="IQ53" s="7"/>
+      <c r="IR53" s="7"/>
+      <c r="IS53" s="7"/>
+      <c r="IT53" s="7"/>
+      <c r="IU53" s="7"/>
     </row>
     <row r="54" spans="1:256">
       <c r="A54">
@@ -4132,7 +4137,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Removable cover for RF shield</t>
+          <t>RF shield with removable cover</t>
         </is>
       </c>
       <c r="E54" t="s">
@@ -4140,639 +4145,630 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
+          <t>BMI-S-202-F</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>903-1051-1-ND</t>
+        </is>
+      </c>
+      <c r="I54">
+        <v>1.79</v>
+      </c>
+      <c r="J54">
+        <v>1.5800000000000001</v>
+      </c>
+      <c r="K54">
+        <v>1.25</v>
+      </c>
+      <c r="M54">
+        <f>IF($D$76*A54&lt;10,$D$76*A54*I54,IF($D$76*A54&lt;100,$D$76*A54*J54,$D$76*A54*K54))</f>
+        <v>5.3700000000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:256">
+      <c r="A55">
+        <v>1</v>
+      </c>
+      <c r="B55" t="s">
+        <v>19</v>
+      </c>
+      <c r="C55" t="s">
+        <v>20</v>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Removable cover for RF shield</t>
+        </is>
+      </c>
+      <c r="E55" t="s">
+        <v>21</v>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
           <t>BMI-S-202-C</t>
         </is>
       </c>
-      <c r="G54" t="inlineStr">
+      <c r="G55" t="inlineStr">
         <is>
           <t>903-1014-ND</t>
         </is>
       </c>
-      <c r="I54">
+      <c r="I55">
         <v>1.3799999999999999</v>
       </c>
-      <c r="J54">
+      <c r="J55">
         <v>12.26</v>
       </c>
-      <c r="K54">
+      <c r="K55">
         <v>0.96899999999999997</v>
       </c>
-      <c r="M54">
-        <f>IF($D$75*A54&lt;10,$D$75*A54*I54,IF($D$75*A54&lt;100,$D$75*A54*J54,$D$75*A54*K54))</f>
+      <c r="M55">
+        <f>IF($D$76*A55&lt;10,$D$76*A55*I55,IF($D$76*A55&lt;100,$D$76*A55*J55,$D$76*A55*K55))</f>
         <v>4.1399999999999997</v>
       </c>
     </row>
-    <row r="55" spans="1:256">
-      <c r="A55" s="11"/>
-      <c r="B55" s="11"/>
-      <c r="C55" s="12"/>
-      <c r="D55" s="11"/>
-      <c r="E55" s="11"/>
-      <c r="F55" s="11"/>
-      <c r="G55" s="11"/>
-      <c r="H55" s="11"/>
-      <c r="I55" s="13"/>
-      <c r="J55" s="13"/>
-      <c r="K55" s="13"/>
-      <c r="L55" s="11"/>
-      <c r="M55" s="13"/>
-      <c r="N55" s="11"/>
-      <c r="O55" s="11"/>
-      <c r="P55" s="11"/>
-      <c r="Q55" s="11"/>
-      <c r="R55" s="11"/>
-      <c r="S55" s="11"/>
-      <c r="T55" s="11"/>
-      <c r="U55" s="11"/>
-      <c r="V55" s="11"/>
-      <c r="W55" s="11"/>
-      <c r="X55" s="11"/>
-      <c r="Y55" s="11"/>
-      <c r="Z55" s="11"/>
-      <c r="AA55" s="11"/>
-      <c r="AB55" s="11"/>
-      <c r="AC55" s="11"/>
-      <c r="AD55" s="11"/>
-      <c r="AE55" s="11"/>
-      <c r="AF55" s="11"/>
-      <c r="AG55" s="11"/>
-      <c r="AH55" s="11"/>
-      <c r="AI55" s="11"/>
-      <c r="AJ55" s="11"/>
-      <c r="AK55" s="11"/>
-      <c r="AL55" s="11"/>
-      <c r="AM55" s="11"/>
-      <c r="AN55" s="11"/>
-      <c r="AO55" s="11"/>
-      <c r="AP55" s="11"/>
-      <c r="AQ55" s="11"/>
-      <c r="AR55" s="11"/>
-      <c r="AS55" s="11"/>
-      <c r="AT55" s="11"/>
-      <c r="AU55" s="11"/>
-      <c r="AV55" s="11"/>
-      <c r="AW55" s="11"/>
-      <c r="AX55" s="11"/>
-      <c r="AY55" s="11"/>
-      <c r="AZ55" s="11"/>
-      <c r="BA55" s="11"/>
-      <c r="BB55" s="11"/>
-      <c r="BC55" s="11"/>
-      <c r="BD55" s="11"/>
-      <c r="BE55" s="11"/>
-      <c r="BF55" s="11"/>
-      <c r="BG55" s="11"/>
-      <c r="BH55" s="11"/>
-      <c r="BI55" s="11"/>
-      <c r="BJ55" s="11"/>
-      <c r="BK55" s="11"/>
-      <c r="BL55" s="11"/>
-      <c r="BM55" s="11"/>
-      <c r="BN55" s="11"/>
-      <c r="BO55" s="11"/>
-      <c r="BP55" s="11"/>
-      <c r="BQ55" s="11"/>
-      <c r="BR55" s="11"/>
-      <c r="BS55" s="11"/>
-      <c r="BT55" s="11"/>
-      <c r="BU55" s="11"/>
-      <c r="BV55" s="11"/>
-      <c r="BW55" s="11"/>
-      <c r="BX55" s="11"/>
-      <c r="BY55" s="11"/>
-      <c r="BZ55" s="11"/>
-      <c r="CA55" s="11"/>
-      <c r="CB55" s="11"/>
-      <c r="CC55" s="11"/>
-      <c r="CD55" s="11"/>
-      <c r="CE55" s="11"/>
-      <c r="CF55" s="11"/>
-      <c r="CG55" s="11"/>
-      <c r="CH55" s="11"/>
-      <c r="CI55" s="11"/>
-      <c r="CJ55" s="11"/>
-      <c r="CK55" s="11"/>
-      <c r="CL55" s="11"/>
-      <c r="CM55" s="11"/>
-      <c r="CN55" s="11"/>
-      <c r="CO55" s="11"/>
-      <c r="CP55" s="11"/>
-      <c r="CQ55" s="11"/>
-      <c r="CR55" s="11"/>
-      <c r="CS55" s="11"/>
-      <c r="CT55" s="11"/>
-      <c r="CU55" s="11"/>
-      <c r="CV55" s="11"/>
-      <c r="CW55" s="11"/>
-      <c r="CX55" s="11"/>
-      <c r="CY55" s="11"/>
-      <c r="CZ55" s="11"/>
-      <c r="DA55" s="11"/>
-      <c r="DB55" s="11"/>
-      <c r="DC55" s="11"/>
-      <c r="DD55" s="11"/>
-      <c r="DE55" s="11"/>
-      <c r="DF55" s="11"/>
-      <c r="DG55" s="11"/>
-      <c r="DH55" s="11"/>
-      <c r="DI55" s="11"/>
-      <c r="DJ55" s="11"/>
-      <c r="DK55" s="11"/>
-      <c r="DL55" s="11"/>
-      <c r="DM55" s="11"/>
-      <c r="DN55" s="11"/>
-      <c r="DO55" s="11"/>
-      <c r="DP55" s="11"/>
-      <c r="DQ55" s="11"/>
-      <c r="DR55" s="11"/>
-      <c r="DS55" s="11"/>
-      <c r="DT55" s="11"/>
-      <c r="DU55" s="11"/>
-      <c r="DV55" s="11"/>
-      <c r="DW55" s="11"/>
-      <c r="DX55" s="11"/>
-      <c r="DY55" s="11"/>
-      <c r="DZ55" s="11"/>
-      <c r="EA55" s="11"/>
-      <c r="EB55" s="11"/>
-      <c r="EC55" s="11"/>
-      <c r="ED55" s="11"/>
-      <c r="EE55" s="11"/>
-      <c r="EF55" s="11"/>
-      <c r="EG55" s="11"/>
-      <c r="EH55" s="11"/>
-      <c r="EI55" s="11"/>
-      <c r="EJ55" s="11"/>
-      <c r="EK55" s="11"/>
-      <c r="EL55" s="11"/>
-      <c r="EM55" s="11"/>
-      <c r="EN55" s="11"/>
-      <c r="EO55" s="11"/>
-      <c r="EP55" s="11"/>
-      <c r="EQ55" s="11"/>
-      <c r="ER55" s="11"/>
-      <c r="ES55" s="11"/>
-      <c r="ET55" s="11"/>
-      <c r="EU55" s="11"/>
-      <c r="EV55" s="11"/>
-      <c r="EW55" s="11"/>
-      <c r="EX55" s="11"/>
-      <c r="EY55" s="11"/>
-      <c r="EZ55" s="11"/>
-      <c r="FA55" s="11"/>
-      <c r="FB55" s="11"/>
-      <c r="FC55" s="11"/>
-      <c r="FD55" s="11"/>
-      <c r="FE55" s="11"/>
-      <c r="FF55" s="11"/>
-      <c r="FG55" s="11"/>
-      <c r="FH55" s="11"/>
-      <c r="FI55" s="11"/>
-      <c r="FJ55" s="11"/>
-      <c r="FK55" s="11"/>
-      <c r="FL55" s="11"/>
-      <c r="FM55" s="11"/>
-      <c r="FN55" s="11"/>
-      <c r="FO55" s="11"/>
-      <c r="FP55" s="11"/>
-      <c r="FQ55" s="11"/>
-      <c r="FR55" s="11"/>
-      <c r="FS55" s="11"/>
-      <c r="FT55" s="11"/>
-      <c r="FU55" s="11"/>
-      <c r="FV55" s="11"/>
-      <c r="FW55" s="11"/>
-      <c r="FX55" s="11"/>
-      <c r="FY55" s="11"/>
-      <c r="FZ55" s="11"/>
-      <c r="GA55" s="11"/>
-      <c r="GB55" s="11"/>
-      <c r="GC55" s="11"/>
-      <c r="GD55" s="11"/>
-      <c r="GE55" s="11"/>
-      <c r="GF55" s="11"/>
-      <c r="GG55" s="11"/>
-      <c r="GH55" s="11"/>
-      <c r="GI55" s="11"/>
-      <c r="GJ55" s="11"/>
-      <c r="GK55" s="11"/>
-      <c r="GL55" s="11"/>
-      <c r="GM55" s="11"/>
-      <c r="GN55" s="11"/>
-      <c r="GO55" s="11"/>
-      <c r="GP55" s="11"/>
-      <c r="GQ55" s="11"/>
-      <c r="GR55" s="11"/>
-      <c r="GS55" s="11"/>
-      <c r="GT55" s="11"/>
-      <c r="GU55" s="11"/>
-      <c r="GV55" s="11"/>
-      <c r="GW55" s="11"/>
-      <c r="GX55" s="11"/>
-      <c r="GY55" s="11"/>
-      <c r="GZ55" s="11"/>
-      <c r="HA55" s="11"/>
-      <c r="HB55" s="11"/>
-      <c r="HC55" s="11"/>
-      <c r="HD55" s="11"/>
-      <c r="HE55" s="11"/>
-      <c r="HF55" s="11"/>
-      <c r="HG55" s="11"/>
-      <c r="HH55" s="11"/>
-      <c r="HI55" s="11"/>
-      <c r="HJ55" s="11"/>
-      <c r="HK55" s="11"/>
-      <c r="HL55" s="11"/>
-      <c r="HM55" s="11"/>
-      <c r="HN55" s="11"/>
-      <c r="HO55" s="11"/>
-      <c r="HP55" s="11"/>
-      <c r="HQ55" s="11"/>
-      <c r="HR55" s="11"/>
-      <c r="HS55" s="11"/>
-      <c r="HT55" s="11"/>
-      <c r="HU55" s="11"/>
-      <c r="HV55" s="11"/>
-      <c r="HW55" s="11"/>
-      <c r="HX55" s="11"/>
-      <c r="HY55" s="11"/>
-      <c r="HZ55" s="11"/>
-      <c r="IA55" s="11"/>
-      <c r="IB55" s="11"/>
-      <c r="IC55" s="11"/>
-      <c r="ID55" s="11"/>
-      <c r="IE55" s="11"/>
-      <c r="IF55" s="11"/>
-      <c r="IG55" s="11"/>
-      <c r="IH55" s="11"/>
-      <c r="II55" s="11"/>
-      <c r="IJ55" s="11"/>
-      <c r="IK55" s="11"/>
-      <c r="IL55" s="11"/>
-      <c r="IM55" s="11"/>
-      <c r="IN55" s="11"/>
-      <c r="IO55" s="11"/>
-      <c r="IP55" s="11"/>
-      <c r="IQ55" s="11"/>
-      <c r="IR55" s="11"/>
-      <c r="IS55" s="11"/>
-      <c r="IT55" s="11"/>
-      <c r="IU55" s="11"/>
-      <c r="IV55" s="14"/>
-    </row>
     <row r="56" spans="1:256">
-      <c r="A56">
+      <c r="A56" s="11"/>
+      <c r="B56" s="11"/>
+      <c r="C56" s="12"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="11"/>
+      <c r="G56" s="11"/>
+      <c r="H56" s="11"/>
+      <c r="I56" s="13"/>
+      <c r="J56" s="13"/>
+      <c r="K56" s="13"/>
+      <c r="L56" s="11"/>
+      <c r="M56" s="13"/>
+      <c r="N56" s="11"/>
+      <c r="O56" s="11"/>
+      <c r="P56" s="11"/>
+      <c r="Q56" s="11"/>
+      <c r="R56" s="11"/>
+      <c r="S56" s="11"/>
+      <c r="T56" s="11"/>
+      <c r="U56" s="11"/>
+      <c r="V56" s="11"/>
+      <c r="W56" s="11"/>
+      <c r="X56" s="11"/>
+      <c r="Y56" s="11"/>
+      <c r="Z56" s="11"/>
+      <c r="AA56" s="11"/>
+      <c r="AB56" s="11"/>
+      <c r="AC56" s="11"/>
+      <c r="AD56" s="11"/>
+      <c r="AE56" s="11"/>
+      <c r="AF56" s="11"/>
+      <c r="AG56" s="11"/>
+      <c r="AH56" s="11"/>
+      <c r="AI56" s="11"/>
+      <c r="AJ56" s="11"/>
+      <c r="AK56" s="11"/>
+      <c r="AL56" s="11"/>
+      <c r="AM56" s="11"/>
+      <c r="AN56" s="11"/>
+      <c r="AO56" s="11"/>
+      <c r="AP56" s="11"/>
+      <c r="AQ56" s="11"/>
+      <c r="AR56" s="11"/>
+      <c r="AS56" s="11"/>
+      <c r="AT56" s="11"/>
+      <c r="AU56" s="11"/>
+      <c r="AV56" s="11"/>
+      <c r="AW56" s="11"/>
+      <c r="AX56" s="11"/>
+      <c r="AY56" s="11"/>
+      <c r="AZ56" s="11"/>
+      <c r="BA56" s="11"/>
+      <c r="BB56" s="11"/>
+      <c r="BC56" s="11"/>
+      <c r="BD56" s="11"/>
+      <c r="BE56" s="11"/>
+      <c r="BF56" s="11"/>
+      <c r="BG56" s="11"/>
+      <c r="BH56" s="11"/>
+      <c r="BI56" s="11"/>
+      <c r="BJ56" s="11"/>
+      <c r="BK56" s="11"/>
+      <c r="BL56" s="11"/>
+      <c r="BM56" s="11"/>
+      <c r="BN56" s="11"/>
+      <c r="BO56" s="11"/>
+      <c r="BP56" s="11"/>
+      <c r="BQ56" s="11"/>
+      <c r="BR56" s="11"/>
+      <c r="BS56" s="11"/>
+      <c r="BT56" s="11"/>
+      <c r="BU56" s="11"/>
+      <c r="BV56" s="11"/>
+      <c r="BW56" s="11"/>
+      <c r="BX56" s="11"/>
+      <c r="BY56" s="11"/>
+      <c r="BZ56" s="11"/>
+      <c r="CA56" s="11"/>
+      <c r="CB56" s="11"/>
+      <c r="CC56" s="11"/>
+      <c r="CD56" s="11"/>
+      <c r="CE56" s="11"/>
+      <c r="CF56" s="11"/>
+      <c r="CG56" s="11"/>
+      <c r="CH56" s="11"/>
+      <c r="CI56" s="11"/>
+      <c r="CJ56" s="11"/>
+      <c r="CK56" s="11"/>
+      <c r="CL56" s="11"/>
+      <c r="CM56" s="11"/>
+      <c r="CN56" s="11"/>
+      <c r="CO56" s="11"/>
+      <c r="CP56" s="11"/>
+      <c r="CQ56" s="11"/>
+      <c r="CR56" s="11"/>
+      <c r="CS56" s="11"/>
+      <c r="CT56" s="11"/>
+      <c r="CU56" s="11"/>
+      <c r="CV56" s="11"/>
+      <c r="CW56" s="11"/>
+      <c r="CX56" s="11"/>
+      <c r="CY56" s="11"/>
+      <c r="CZ56" s="11"/>
+      <c r="DA56" s="11"/>
+      <c r="DB56" s="11"/>
+      <c r="DC56" s="11"/>
+      <c r="DD56" s="11"/>
+      <c r="DE56" s="11"/>
+      <c r="DF56" s="11"/>
+      <c r="DG56" s="11"/>
+      <c r="DH56" s="11"/>
+      <c r="DI56" s="11"/>
+      <c r="DJ56" s="11"/>
+      <c r="DK56" s="11"/>
+      <c r="DL56" s="11"/>
+      <c r="DM56" s="11"/>
+      <c r="DN56" s="11"/>
+      <c r="DO56" s="11"/>
+      <c r="DP56" s="11"/>
+      <c r="DQ56" s="11"/>
+      <c r="DR56" s="11"/>
+      <c r="DS56" s="11"/>
+      <c r="DT56" s="11"/>
+      <c r="DU56" s="11"/>
+      <c r="DV56" s="11"/>
+      <c r="DW56" s="11"/>
+      <c r="DX56" s="11"/>
+      <c r="DY56" s="11"/>
+      <c r="DZ56" s="11"/>
+      <c r="EA56" s="11"/>
+      <c r="EB56" s="11"/>
+      <c r="EC56" s="11"/>
+      <c r="ED56" s="11"/>
+      <c r="EE56" s="11"/>
+      <c r="EF56" s="11"/>
+      <c r="EG56" s="11"/>
+      <c r="EH56" s="11"/>
+      <c r="EI56" s="11"/>
+      <c r="EJ56" s="11"/>
+      <c r="EK56" s="11"/>
+      <c r="EL56" s="11"/>
+      <c r="EM56" s="11"/>
+      <c r="EN56" s="11"/>
+      <c r="EO56" s="11"/>
+      <c r="EP56" s="11"/>
+      <c r="EQ56" s="11"/>
+      <c r="ER56" s="11"/>
+      <c r="ES56" s="11"/>
+      <c r="ET56" s="11"/>
+      <c r="EU56" s="11"/>
+      <c r="EV56" s="11"/>
+      <c r="EW56" s="11"/>
+      <c r="EX56" s="11"/>
+      <c r="EY56" s="11"/>
+      <c r="EZ56" s="11"/>
+      <c r="FA56" s="11"/>
+      <c r="FB56" s="11"/>
+      <c r="FC56" s="11"/>
+      <c r="FD56" s="11"/>
+      <c r="FE56" s="11"/>
+      <c r="FF56" s="11"/>
+      <c r="FG56" s="11"/>
+      <c r="FH56" s="11"/>
+      <c r="FI56" s="11"/>
+      <c r="FJ56" s="11"/>
+      <c r="FK56" s="11"/>
+      <c r="FL56" s="11"/>
+      <c r="FM56" s="11"/>
+      <c r="FN56" s="11"/>
+      <c r="FO56" s="11"/>
+      <c r="FP56" s="11"/>
+      <c r="FQ56" s="11"/>
+      <c r="FR56" s="11"/>
+      <c r="FS56" s="11"/>
+      <c r="FT56" s="11"/>
+      <c r="FU56" s="11"/>
+      <c r="FV56" s="11"/>
+      <c r="FW56" s="11"/>
+      <c r="FX56" s="11"/>
+      <c r="FY56" s="11"/>
+      <c r="FZ56" s="11"/>
+      <c r="GA56" s="11"/>
+      <c r="GB56" s="11"/>
+      <c r="GC56" s="11"/>
+      <c r="GD56" s="11"/>
+      <c r="GE56" s="11"/>
+      <c r="GF56" s="11"/>
+      <c r="GG56" s="11"/>
+      <c r="GH56" s="11"/>
+      <c r="GI56" s="11"/>
+      <c r="GJ56" s="11"/>
+      <c r="GK56" s="11"/>
+      <c r="GL56" s="11"/>
+      <c r="GM56" s="11"/>
+      <c r="GN56" s="11"/>
+      <c r="GO56" s="11"/>
+      <c r="GP56" s="11"/>
+      <c r="GQ56" s="11"/>
+      <c r="GR56" s="11"/>
+      <c r="GS56" s="11"/>
+      <c r="GT56" s="11"/>
+      <c r="GU56" s="11"/>
+      <c r="GV56" s="11"/>
+      <c r="GW56" s="11"/>
+      <c r="GX56" s="11"/>
+      <c r="GY56" s="11"/>
+      <c r="GZ56" s="11"/>
+      <c r="HA56" s="11"/>
+      <c r="HB56" s="11"/>
+      <c r="HC56" s="11"/>
+      <c r="HD56" s="11"/>
+      <c r="HE56" s="11"/>
+      <c r="HF56" s="11"/>
+      <c r="HG56" s="11"/>
+      <c r="HH56" s="11"/>
+      <c r="HI56" s="11"/>
+      <c r="HJ56" s="11"/>
+      <c r="HK56" s="11"/>
+      <c r="HL56" s="11"/>
+      <c r="HM56" s="11"/>
+      <c r="HN56" s="11"/>
+      <c r="HO56" s="11"/>
+      <c r="HP56" s="11"/>
+      <c r="HQ56" s="11"/>
+      <c r="HR56" s="11"/>
+      <c r="HS56" s="11"/>
+      <c r="HT56" s="11"/>
+      <c r="HU56" s="11"/>
+      <c r="HV56" s="11"/>
+      <c r="HW56" s="11"/>
+      <c r="HX56" s="11"/>
+      <c r="HY56" s="11"/>
+      <c r="HZ56" s="11"/>
+      <c r="IA56" s="11"/>
+      <c r="IB56" s="11"/>
+      <c r="IC56" s="11"/>
+      <c r="ID56" s="11"/>
+      <c r="IE56" s="11"/>
+      <c r="IF56" s="11"/>
+      <c r="IG56" s="11"/>
+      <c r="IH56" s="11"/>
+      <c r="II56" s="11"/>
+      <c r="IJ56" s="11"/>
+      <c r="IK56" s="11"/>
+      <c r="IL56" s="11"/>
+      <c r="IM56" s="11"/>
+      <c r="IN56" s="11"/>
+      <c r="IO56" s="11"/>
+      <c r="IP56" s="11"/>
+      <c r="IQ56" s="11"/>
+      <c r="IR56" s="11"/>
+      <c r="IS56" s="11"/>
+      <c r="IT56" s="11"/>
+      <c r="IU56" s="11"/>
+      <c r="IV56" s="14"/>
+    </row>
+    <row r="57" spans="1:256">
+      <c r="A57">
         <v>2</v>
       </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>T1, T2</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>T1,T2</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
         <is>
           <t>ALT4532</t>
         </is>
       </c>
-      <c r="D56" t="inlineStr">
+      <c r="D57" t="inlineStr">
         <is>
           <t>Mini Ethernet transformer</t>
         </is>
       </c>
-      <c r="E56" t="s">
+      <c r="E57" t="s">
         <v>2</v>
       </c>
-      <c r="F56" t="inlineStr">
+      <c r="F57" t="inlineStr">
         <is>
           <t>ALT4532M-201-T001</t>
         </is>
       </c>
-      <c r="G56" t="inlineStr">
+      <c r="G57" t="inlineStr">
         <is>
           <t>445-15085-1-ND</t>
         </is>
       </c>
-      <c r="I56">
+      <c r="I57">
         <v>1.49</v>
       </c>
-      <c r="J56">
+      <c r="J57">
         <v>1.1899999999999999</v>
       </c>
-      <c r="K56">
+      <c r="K57">
         <v>0.92000000000000004</v>
       </c>
-      <c r="M56">
-        <f>IF($D$75*A56&lt;10,$D$75*A56*I56,IF($D$75*A56&lt;100,$D$75*A56*J56,$D$75*A56*K56))</f>
+      <c r="M57">
+        <f>IF($D$76*A57&lt;10,$D$76*A57*I57,IF($D$76*A57&lt;100,$D$76*A57*J57,$D$76*A57*K57))</f>
         <v>8.9399999999999995</v>
       </c>
     </row>
-    <row r="57" spans="1:256">
-      <c r="A57" s="7"/>
-      <c r="B57" s="7"/>
-      <c r="C57" s="8"/>
-      <c r="D57" s="7"/>
-      <c r="E57" s="7"/>
-      <c r="F57" s="7"/>
-      <c r="G57" s="7"/>
-      <c r="H57" s="7"/>
-      <c r="I57" s="9"/>
-      <c r="J57" s="9"/>
-      <c r="K57" s="9"/>
-      <c r="L57" s="7"/>
-      <c r="M57" s="9"/>
-      <c r="N57" s="7"/>
-      <c r="O57" s="7"/>
-      <c r="P57" s="7"/>
-      <c r="Q57" s="7"/>
-      <c r="R57" s="7"/>
-      <c r="S57" s="7"/>
-      <c r="T57" s="7"/>
-      <c r="U57" s="7"/>
-      <c r="V57" s="7"/>
-      <c r="W57" s="7"/>
-      <c r="X57" s="7"/>
-      <c r="Y57" s="7"/>
-      <c r="Z57" s="7"/>
-      <c r="AA57" s="7"/>
-      <c r="AB57" s="7"/>
-      <c r="AC57" s="7"/>
-      <c r="AD57" s="7"/>
-      <c r="AE57" s="7"/>
-      <c r="AF57" s="7"/>
-      <c r="AG57" s="7"/>
-      <c r="AH57" s="7"/>
-      <c r="AI57" s="7"/>
-      <c r="AJ57" s="7"/>
-      <c r="AK57" s="7"/>
-      <c r="AL57" s="7"/>
-      <c r="AM57" s="7"/>
-      <c r="AN57" s="7"/>
-      <c r="AO57" s="7"/>
-      <c r="AP57" s="7"/>
-      <c r="AQ57" s="7"/>
-      <c r="AR57" s="7"/>
-      <c r="AS57" s="7"/>
-      <c r="AT57" s="7"/>
-      <c r="AU57" s="7"/>
-      <c r="AV57" s="7"/>
-      <c r="AW57" s="7"/>
-      <c r="AX57" s="7"/>
-      <c r="AY57" s="7"/>
-      <c r="AZ57" s="7"/>
-      <c r="BA57" s="7"/>
-      <c r="BB57" s="7"/>
-      <c r="BC57" s="7"/>
-      <c r="BD57" s="7"/>
-      <c r="BE57" s="7"/>
-      <c r="BF57" s="7"/>
-      <c r="BG57" s="7"/>
-      <c r="BH57" s="7"/>
-      <c r="BI57" s="7"/>
-      <c r="BJ57" s="7"/>
-      <c r="BK57" s="7"/>
-      <c r="BL57" s="7"/>
-      <c r="BM57" s="7"/>
-      <c r="BN57" s="7"/>
-      <c r="BO57" s="7"/>
-      <c r="BP57" s="7"/>
-      <c r="BQ57" s="7"/>
-      <c r="BR57" s="7"/>
-      <c r="BS57" s="7"/>
-      <c r="BT57" s="7"/>
-      <c r="BU57" s="7"/>
-      <c r="BV57" s="7"/>
-      <c r="BW57" s="7"/>
-      <c r="BX57" s="7"/>
-      <c r="BY57" s="7"/>
-      <c r="BZ57" s="7"/>
-      <c r="CA57" s="7"/>
-      <c r="CB57" s="7"/>
-      <c r="CC57" s="7"/>
-      <c r="CD57" s="7"/>
-      <c r="CE57" s="7"/>
-      <c r="CF57" s="7"/>
-      <c r="CG57" s="7"/>
-      <c r="CH57" s="7"/>
-      <c r="CI57" s="7"/>
-      <c r="CJ57" s="7"/>
-      <c r="CK57" s="7"/>
-      <c r="CL57" s="7"/>
-      <c r="CM57" s="7"/>
-      <c r="CN57" s="7"/>
-      <c r="CO57" s="7"/>
-      <c r="CP57" s="7"/>
-      <c r="CQ57" s="7"/>
-      <c r="CR57" s="7"/>
-      <c r="CS57" s="7"/>
-      <c r="CT57" s="7"/>
-      <c r="CU57" s="7"/>
-      <c r="CV57" s="7"/>
-      <c r="CW57" s="7"/>
-      <c r="CX57" s="7"/>
-      <c r="CY57" s="7"/>
-      <c r="CZ57" s="7"/>
-      <c r="DA57" s="7"/>
-      <c r="DB57" s="7"/>
-      <c r="DC57" s="7"/>
-      <c r="DD57" s="7"/>
-      <c r="DE57" s="7"/>
-      <c r="DF57" s="7"/>
-      <c r="DG57" s="7"/>
-      <c r="DH57" s="7"/>
-      <c r="DI57" s="7"/>
-      <c r="DJ57" s="7"/>
-      <c r="DK57" s="7"/>
-      <c r="DL57" s="7"/>
-      <c r="DM57" s="7"/>
-      <c r="DN57" s="7"/>
-      <c r="DO57" s="7"/>
-      <c r="DP57" s="7"/>
-      <c r="DQ57" s="7"/>
-      <c r="DR57" s="7"/>
-      <c r="DS57" s="7"/>
-      <c r="DT57" s="7"/>
-      <c r="DU57" s="7"/>
-      <c r="DV57" s="7"/>
-      <c r="DW57" s="7"/>
-      <c r="DX57" s="7"/>
-      <c r="DY57" s="7"/>
-      <c r="DZ57" s="7"/>
-      <c r="EA57" s="7"/>
-      <c r="EB57" s="7"/>
-      <c r="EC57" s="7"/>
-      <c r="ED57" s="7"/>
-      <c r="EE57" s="7"/>
-      <c r="EF57" s="7"/>
-      <c r="EG57" s="7"/>
-      <c r="EH57" s="7"/>
-      <c r="EI57" s="7"/>
-      <c r="EJ57" s="7"/>
-      <c r="EK57" s="7"/>
-      <c r="EL57" s="7"/>
-      <c r="EM57" s="7"/>
-      <c r="EN57" s="7"/>
-      <c r="EO57" s="7"/>
-      <c r="EP57" s="7"/>
-      <c r="EQ57" s="7"/>
-      <c r="ER57" s="7"/>
-      <c r="ES57" s="7"/>
-      <c r="ET57" s="7"/>
-      <c r="EU57" s="7"/>
-      <c r="EV57" s="7"/>
-      <c r="EW57" s="7"/>
-      <c r="EX57" s="7"/>
-      <c r="EY57" s="7"/>
-      <c r="EZ57" s="7"/>
-      <c r="FA57" s="7"/>
-      <c r="FB57" s="7"/>
-      <c r="FC57" s="7"/>
-      <c r="FD57" s="7"/>
-      <c r="FE57" s="7"/>
-      <c r="FF57" s="7"/>
-      <c r="FG57" s="7"/>
-      <c r="FH57" s="7"/>
-      <c r="FI57" s="7"/>
-      <c r="FJ57" s="7"/>
-      <c r="FK57" s="7"/>
-      <c r="FL57" s="7"/>
-      <c r="FM57" s="7"/>
-      <c r="FN57" s="7"/>
-      <c r="FO57" s="7"/>
-      <c r="FP57" s="7"/>
-      <c r="FQ57" s="7"/>
-      <c r="FR57" s="7"/>
-      <c r="FS57" s="7"/>
-      <c r="FT57" s="7"/>
-      <c r="FU57" s="7"/>
-      <c r="FV57" s="7"/>
-      <c r="FW57" s="7"/>
-      <c r="FX57" s="7"/>
-      <c r="FY57" s="7"/>
-      <c r="FZ57" s="7"/>
-      <c r="GA57" s="7"/>
-      <c r="GB57" s="7"/>
-      <c r="GC57" s="7"/>
-      <c r="GD57" s="7"/>
-      <c r="GE57" s="7"/>
-      <c r="GF57" s="7"/>
-      <c r="GG57" s="7"/>
-      <c r="GH57" s="7"/>
-      <c r="GI57" s="7"/>
-      <c r="GJ57" s="7"/>
-      <c r="GK57" s="7"/>
-      <c r="GL57" s="7"/>
-      <c r="GM57" s="7"/>
-      <c r="GN57" s="7"/>
-      <c r="GO57" s="7"/>
-      <c r="GP57" s="7"/>
-      <c r="GQ57" s="7"/>
-      <c r="GR57" s="7"/>
-      <c r="GS57" s="7"/>
-      <c r="GT57" s="7"/>
-      <c r="GU57" s="7"/>
-      <c r="GV57" s="7"/>
-      <c r="GW57" s="7"/>
-      <c r="GX57" s="7"/>
-      <c r="GY57" s="7"/>
-      <c r="GZ57" s="7"/>
-      <c r="HA57" s="7"/>
-      <c r="HB57" s="7"/>
-      <c r="HC57" s="7"/>
-      <c r="HD57" s="7"/>
-      <c r="HE57" s="7"/>
-      <c r="HF57" s="7"/>
-      <c r="HG57" s="7"/>
-      <c r="HH57" s="7"/>
-      <c r="HI57" s="7"/>
-      <c r="HJ57" s="7"/>
-      <c r="HK57" s="7"/>
-      <c r="HL57" s="7"/>
-      <c r="HM57" s="7"/>
-      <c r="HN57" s="7"/>
-      <c r="HO57" s="7"/>
-      <c r="HP57" s="7"/>
-      <c r="HQ57" s="7"/>
-      <c r="HR57" s="7"/>
-      <c r="HS57" s="7"/>
-      <c r="HT57" s="7"/>
-      <c r="HU57" s="7"/>
-      <c r="HV57" s="7"/>
-      <c r="HW57" s="7"/>
-      <c r="HX57" s="7"/>
-      <c r="HY57" s="7"/>
-      <c r="HZ57" s="7"/>
-      <c r="IA57" s="7"/>
-      <c r="IB57" s="7"/>
-      <c r="IC57" s="7"/>
-      <c r="ID57" s="7"/>
-      <c r="IE57" s="7"/>
-      <c r="IF57" s="7"/>
-      <c r="IG57" s="7"/>
-      <c r="IH57" s="7"/>
-      <c r="II57" s="7"/>
-      <c r="IJ57" s="7"/>
-      <c r="IK57" s="7"/>
-      <c r="IL57" s="7"/>
-      <c r="IM57" s="7"/>
-      <c r="IN57" s="7"/>
-      <c r="IO57" s="7"/>
-      <c r="IP57" s="7"/>
-      <c r="IQ57" s="7"/>
-      <c r="IR57" s="7"/>
-      <c r="IS57" s="7"/>
-      <c r="IT57" s="7"/>
-      <c r="IU57" s="7"/>
-    </row>
     <row r="58" spans="1:256">
-      <c r="A58">
-        <v>1</v>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>U1</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>MAX2769</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>GPS receiver Front End</t>
-        </is>
-      </c>
-      <c r="E58" t="s">
-        <v>22</v>
-      </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>MAX2769ETI+</t>
-        </is>
-      </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>MAX2769ETI+T-ND</t>
-        </is>
-      </c>
-      <c r="H58" t="inlineStr">
-        <is>
-          <t>Mouser 700-MAX2769ETI+</t>
-        </is>
-      </c>
-      <c r="I58">
-        <v>7.1500000000000004</v>
-      </c>
-      <c r="J58">
-        <v>6.5</v>
-      </c>
-      <c r="K58">
-        <v>4.8799999999999999</v>
-      </c>
-      <c r="M58">
-        <f>IF($D$75*A58&lt;10,$D$75*A58*I58,IF($D$75*A58&lt;100,$D$75*A58*J58,$D$75*A58*K58))</f>
-        <v>21.450000000000003</v>
-      </c>
+      <c r="A58" s="7"/>
+      <c r="B58" s="7"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="7"/>
+      <c r="E58" s="7"/>
+      <c r="F58" s="7"/>
+      <c r="G58" s="7"/>
+      <c r="H58" s="7"/>
+      <c r="I58" s="9"/>
+      <c r="J58" s="9"/>
+      <c r="K58" s="9"/>
+      <c r="L58" s="7"/>
+      <c r="M58" s="9"/>
+      <c r="N58" s="7"/>
+      <c r="O58" s="7"/>
+      <c r="P58" s="7"/>
+      <c r="Q58" s="7"/>
+      <c r="R58" s="7"/>
+      <c r="S58" s="7"/>
+      <c r="T58" s="7"/>
+      <c r="U58" s="7"/>
+      <c r="V58" s="7"/>
+      <c r="W58" s="7"/>
+      <c r="X58" s="7"/>
+      <c r="Y58" s="7"/>
+      <c r="Z58" s="7"/>
+      <c r="AA58" s="7"/>
+      <c r="AB58" s="7"/>
+      <c r="AC58" s="7"/>
+      <c r="AD58" s="7"/>
+      <c r="AE58" s="7"/>
+      <c r="AF58" s="7"/>
+      <c r="AG58" s="7"/>
+      <c r="AH58" s="7"/>
+      <c r="AI58" s="7"/>
+      <c r="AJ58" s="7"/>
+      <c r="AK58" s="7"/>
+      <c r="AL58" s="7"/>
+      <c r="AM58" s="7"/>
+      <c r="AN58" s="7"/>
+      <c r="AO58" s="7"/>
+      <c r="AP58" s="7"/>
+      <c r="AQ58" s="7"/>
+      <c r="AR58" s="7"/>
+      <c r="AS58" s="7"/>
+      <c r="AT58" s="7"/>
+      <c r="AU58" s="7"/>
+      <c r="AV58" s="7"/>
+      <c r="AW58" s="7"/>
+      <c r="AX58" s="7"/>
+      <c r="AY58" s="7"/>
+      <c r="AZ58" s="7"/>
+      <c r="BA58" s="7"/>
+      <c r="BB58" s="7"/>
+      <c r="BC58" s="7"/>
+      <c r="BD58" s="7"/>
+      <c r="BE58" s="7"/>
+      <c r="BF58" s="7"/>
+      <c r="BG58" s="7"/>
+      <c r="BH58" s="7"/>
+      <c r="BI58" s="7"/>
+      <c r="BJ58" s="7"/>
+      <c r="BK58" s="7"/>
+      <c r="BL58" s="7"/>
+      <c r="BM58" s="7"/>
+      <c r="BN58" s="7"/>
+      <c r="BO58" s="7"/>
+      <c r="BP58" s="7"/>
+      <c r="BQ58" s="7"/>
+      <c r="BR58" s="7"/>
+      <c r="BS58" s="7"/>
+      <c r="BT58" s="7"/>
+      <c r="BU58" s="7"/>
+      <c r="BV58" s="7"/>
+      <c r="BW58" s="7"/>
+      <c r="BX58" s="7"/>
+      <c r="BY58" s="7"/>
+      <c r="BZ58" s="7"/>
+      <c r="CA58" s="7"/>
+      <c r="CB58" s="7"/>
+      <c r="CC58" s="7"/>
+      <c r="CD58" s="7"/>
+      <c r="CE58" s="7"/>
+      <c r="CF58" s="7"/>
+      <c r="CG58" s="7"/>
+      <c r="CH58" s="7"/>
+      <c r="CI58" s="7"/>
+      <c r="CJ58" s="7"/>
+      <c r="CK58" s="7"/>
+      <c r="CL58" s="7"/>
+      <c r="CM58" s="7"/>
+      <c r="CN58" s="7"/>
+      <c r="CO58" s="7"/>
+      <c r="CP58" s="7"/>
+      <c r="CQ58" s="7"/>
+      <c r="CR58" s="7"/>
+      <c r="CS58" s="7"/>
+      <c r="CT58" s="7"/>
+      <c r="CU58" s="7"/>
+      <c r="CV58" s="7"/>
+      <c r="CW58" s="7"/>
+      <c r="CX58" s="7"/>
+      <c r="CY58" s="7"/>
+      <c r="CZ58" s="7"/>
+      <c r="DA58" s="7"/>
+      <c r="DB58" s="7"/>
+      <c r="DC58" s="7"/>
+      <c r="DD58" s="7"/>
+      <c r="DE58" s="7"/>
+      <c r="DF58" s="7"/>
+      <c r="DG58" s="7"/>
+      <c r="DH58" s="7"/>
+      <c r="DI58" s="7"/>
+      <c r="DJ58" s="7"/>
+      <c r="DK58" s="7"/>
+      <c r="DL58" s="7"/>
+      <c r="DM58" s="7"/>
+      <c r="DN58" s="7"/>
+      <c r="DO58" s="7"/>
+      <c r="DP58" s="7"/>
+      <c r="DQ58" s="7"/>
+      <c r="DR58" s="7"/>
+      <c r="DS58" s="7"/>
+      <c r="DT58" s="7"/>
+      <c r="DU58" s="7"/>
+      <c r="DV58" s="7"/>
+      <c r="DW58" s="7"/>
+      <c r="DX58" s="7"/>
+      <c r="DY58" s="7"/>
+      <c r="DZ58" s="7"/>
+      <c r="EA58" s="7"/>
+      <c r="EB58" s="7"/>
+      <c r="EC58" s="7"/>
+      <c r="ED58" s="7"/>
+      <c r="EE58" s="7"/>
+      <c r="EF58" s="7"/>
+      <c r="EG58" s="7"/>
+      <c r="EH58" s="7"/>
+      <c r="EI58" s="7"/>
+      <c r="EJ58" s="7"/>
+      <c r="EK58" s="7"/>
+      <c r="EL58" s="7"/>
+      <c r="EM58" s="7"/>
+      <c r="EN58" s="7"/>
+      <c r="EO58" s="7"/>
+      <c r="EP58" s="7"/>
+      <c r="EQ58" s="7"/>
+      <c r="ER58" s="7"/>
+      <c r="ES58" s="7"/>
+      <c r="ET58" s="7"/>
+      <c r="EU58" s="7"/>
+      <c r="EV58" s="7"/>
+      <c r="EW58" s="7"/>
+      <c r="EX58" s="7"/>
+      <c r="EY58" s="7"/>
+      <c r="EZ58" s="7"/>
+      <c r="FA58" s="7"/>
+      <c r="FB58" s="7"/>
+      <c r="FC58" s="7"/>
+      <c r="FD58" s="7"/>
+      <c r="FE58" s="7"/>
+      <c r="FF58" s="7"/>
+      <c r="FG58" s="7"/>
+      <c r="FH58" s="7"/>
+      <c r="FI58" s="7"/>
+      <c r="FJ58" s="7"/>
+      <c r="FK58" s="7"/>
+      <c r="FL58" s="7"/>
+      <c r="FM58" s="7"/>
+      <c r="FN58" s="7"/>
+      <c r="FO58" s="7"/>
+      <c r="FP58" s="7"/>
+      <c r="FQ58" s="7"/>
+      <c r="FR58" s="7"/>
+      <c r="FS58" s="7"/>
+      <c r="FT58" s="7"/>
+      <c r="FU58" s="7"/>
+      <c r="FV58" s="7"/>
+      <c r="FW58" s="7"/>
+      <c r="FX58" s="7"/>
+      <c r="FY58" s="7"/>
+      <c r="FZ58" s="7"/>
+      <c r="GA58" s="7"/>
+      <c r="GB58" s="7"/>
+      <c r="GC58" s="7"/>
+      <c r="GD58" s="7"/>
+      <c r="GE58" s="7"/>
+      <c r="GF58" s="7"/>
+      <c r="GG58" s="7"/>
+      <c r="GH58" s="7"/>
+      <c r="GI58" s="7"/>
+      <c r="GJ58" s="7"/>
+      <c r="GK58" s="7"/>
+      <c r="GL58" s="7"/>
+      <c r="GM58" s="7"/>
+      <c r="GN58" s="7"/>
+      <c r="GO58" s="7"/>
+      <c r="GP58" s="7"/>
+      <c r="GQ58" s="7"/>
+      <c r="GR58" s="7"/>
+      <c r="GS58" s="7"/>
+      <c r="GT58" s="7"/>
+      <c r="GU58" s="7"/>
+      <c r="GV58" s="7"/>
+      <c r="GW58" s="7"/>
+      <c r="GX58" s="7"/>
+      <c r="GY58" s="7"/>
+      <c r="GZ58" s="7"/>
+      <c r="HA58" s="7"/>
+      <c r="HB58" s="7"/>
+      <c r="HC58" s="7"/>
+      <c r="HD58" s="7"/>
+      <c r="HE58" s="7"/>
+      <c r="HF58" s="7"/>
+      <c r="HG58" s="7"/>
+      <c r="HH58" s="7"/>
+      <c r="HI58" s="7"/>
+      <c r="HJ58" s="7"/>
+      <c r="HK58" s="7"/>
+      <c r="HL58" s="7"/>
+      <c r="HM58" s="7"/>
+      <c r="HN58" s="7"/>
+      <c r="HO58" s="7"/>
+      <c r="HP58" s="7"/>
+      <c r="HQ58" s="7"/>
+      <c r="HR58" s="7"/>
+      <c r="HS58" s="7"/>
+      <c r="HT58" s="7"/>
+      <c r="HU58" s="7"/>
+      <c r="HV58" s="7"/>
+      <c r="HW58" s="7"/>
+      <c r="HX58" s="7"/>
+      <c r="HY58" s="7"/>
+      <c r="HZ58" s="7"/>
+      <c r="IA58" s="7"/>
+      <c r="IB58" s="7"/>
+      <c r="IC58" s="7"/>
+      <c r="ID58" s="7"/>
+      <c r="IE58" s="7"/>
+      <c r="IF58" s="7"/>
+      <c r="IG58" s="7"/>
+      <c r="IH58" s="7"/>
+      <c r="II58" s="7"/>
+      <c r="IJ58" s="7"/>
+      <c r="IK58" s="7"/>
+      <c r="IL58" s="7"/>
+      <c r="IM58" s="7"/>
+      <c r="IN58" s="7"/>
+      <c r="IO58" s="7"/>
+      <c r="IP58" s="7"/>
+      <c r="IQ58" s="7"/>
+      <c r="IR58" s="7"/>
+      <c r="IS58" s="7"/>
+      <c r="IT58" s="7"/>
+      <c r="IU58" s="7"/>
     </row>
     <row r="59" spans="1:256">
       <c r="A59">
@@ -4780,46 +4776,49 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>U2</t>
+          <t>U1</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>STM32F407VG</t>
+          <t>MAX2769</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>CORTEX-M4 uC, 100 pin LQFP</t>
-        </is>
-      </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>ST</t>
-        </is>
+          <t>GPS receiver Front End</t>
+        </is>
+      </c>
+      <c r="E59" t="s">
+        <v>22</v>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>STM32F407VGT6</t>
+          <t>MAX2769ETI+</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>497-11605-ND</t>
+          <t>MAX2769ETI+T-ND</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>Mouser 700-MAX2769ETI+</t>
         </is>
       </c>
       <c r="I59">
-        <v>12.779999999999999</v>
+        <v>7.1500000000000004</v>
       </c>
       <c r="J59">
-        <v>11.622</v>
+        <v>6.5</v>
       </c>
       <c r="K59">
-        <v>9.8780000000000001</v>
+        <v>4.8799999999999999</v>
       </c>
       <c r="M59">
-        <f>IF($D$75*A59&lt;10,$D$75*A59*I59,IF($D$75*A59&lt;100,$D$75*A59*J59,$D$75*A59*K59))</f>
-        <v>38.339999999999996</v>
+        <f>IF($D$76*A59&lt;10,$D$76*A59*I59,IF($D$76*A59&lt;100,$D$76*A59*J59,$D$76*A59*K59))</f>
+        <v>21.450000000000003</v>
       </c>
     </row>
     <row r="60" spans="1:256">
@@ -4828,44 +4827,46 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>U3</t>
+          <t>U2</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>KSZ8081</t>
+          <t>STM32F407VG</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Ethernet PHY</t>
-        </is>
-      </c>
-      <c r="E60" t="s">
-        <v>23</v>
+          <t>CORTEX-M4 uC, 100 pin LQFP</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>ST</t>
+        </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>KSZ8081RNDCA TR</t>
+          <t>STM32F407VGT6</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>576-4177-1-ND</t>
+          <t>497-11605-ND</t>
         </is>
       </c>
       <c r="I60">
-        <v>1.52</v>
+        <v>12.779999999999999</v>
       </c>
       <c r="J60">
-        <v>13.4</v>
+        <v>11.622</v>
       </c>
       <c r="K60">
-        <v>1.0584</v>
+        <v>9.8780000000000001</v>
       </c>
       <c r="M60">
-        <f>IF($D$75*A60&lt;10,$D$75*A60*I60,IF($D$75*A60&lt;100,$D$75*A60*J60,$D$75*A60*K60))</f>
-        <v>4.5600000000000005</v>
+        <f>IF($D$76*A60&lt;10,$D$76*A60*I60,IF($D$76*A60&lt;100,$D$76*A60*J60,$D$76*A60*K60))</f>
+        <v>38.339999999999996</v>
       </c>
     </row>
     <row r="61" spans="1:256">
@@ -4874,40 +4875,44 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>U4</t>
-        </is>
-      </c>
-      <c r="C61" t="s">
-        <v>24</v>
+          <t>U3</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>KSZ8081</t>
+        </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>16.386Mhz TCXO, ? PPM</t>
+          <t>Ethernet PHY</t>
         </is>
       </c>
       <c r="E61" t="s">
-        <v>25</v>
-      </c>
-      <c r="F61" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>KSZ8081RNDCA TR</t>
+        </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>887-1548-1-ND</t>
+          <t>576-4177-1-ND</t>
         </is>
       </c>
       <c r="I61">
-        <v>3.5800000000000001</v>
+        <v>1.52</v>
       </c>
       <c r="J61">
-        <v>3.4020000000000001</v>
+        <v>13.4</v>
       </c>
       <c r="K61">
-        <v>2.899</v>
+        <v>1.0584</v>
       </c>
       <c r="M61">
-        <f>IF($D$75*A61&lt;10,$D$75*A61*I61,IF($D$75*A61&lt;100,$D$75*A61*J61,$D$75*A61*K61))</f>
-        <v>10.74</v>
+        <f>IF($D$76*A61&lt;10,$D$76*A61*I61,IF($D$76*A61&lt;100,$D$76*A61*J61,$D$76*A61*K61))</f>
+        <v>4.5600000000000005</v>
       </c>
     </row>
     <row r="62" spans="1:256">
@@ -4916,132 +4921,130 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>U5</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>LT1719S6</t>
-        </is>
+          <t>U4</t>
+        </is>
+      </c>
+      <c r="C62" t="s">
+        <v>24</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Fast push/pull comparator</t>
-        </is>
-      </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>Linear</t>
-        </is>
-      </c>
-      <c r="F62" t="inlineStr">
-        <is>
-          <t>LT1719CS6#TRMPBF</t>
-        </is>
+          <t>16.386Mhz TCXO, ? PPM</t>
+        </is>
+      </c>
+      <c r="E62" t="s">
+        <v>25</v>
+      </c>
+      <c r="F62" t="s">
+        <v>24</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>LT1719CS6#TRMPBFCT-ND</t>
+          <t>887-1548-1-ND</t>
         </is>
       </c>
       <c r="I62">
-        <v>3.4900000000000002</v>
+        <v>3.5800000000000001</v>
       </c>
       <c r="J62">
-        <v>3.1099999999999999</v>
+        <v>3.4020000000000001</v>
       </c>
       <c r="K62">
-        <v>2.7999999999999998</v>
+        <v>2.899</v>
       </c>
       <c r="M62">
-        <f>IF($D$75*A62&lt;10,$D$75*A62*I62,IF($D$75*A62&lt;100,$D$75*A62*J62,$D$75*A62*K62))</f>
-        <v>10.470000000000001</v>
+        <f>IF($D$76*A62&lt;10,$D$76*A62*I62,IF($D$76*A62&lt;100,$D$76*A62*J62,$D$76*A62*K62))</f>
+        <v>10.74</v>
       </c>
     </row>
     <row r="63" spans="1:256">
       <c r="A63">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>U6, U7, U11</t>
-        </is>
-      </c>
-      <c r="C63" t="s">
-        <v>26</v>
+          <t>U5</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>LT1719S6</t>
+        </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>2.85V low noise LDO</t>
-        </is>
-      </c>
-      <c r="E63" t="s">
-        <v>22</v>
-      </c>
-      <c r="F63" t="s">
-        <v>26</v>
+          <t>Fast push/pull comparator</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Linear</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>LT1719CS6#TRMPBF</t>
+        </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>MAX8510EXK29+TCT-ND</t>
+          <t>LT1719CS6#TRMPBFCT-ND</t>
         </is>
       </c>
       <c r="I63">
-        <v>1.22</v>
+        <v>3.4900000000000002</v>
       </c>
       <c r="J63">
-        <v>1.1499999999999999</v>
+        <v>3.1099999999999999</v>
       </c>
       <c r="K63">
-        <v>0.80300000000000005</v>
+        <v>2.7999999999999998</v>
       </c>
       <c r="M63">
-        <f>IF($D$75*A63&lt;10,$D$75*A63*I63,IF($D$75*A63&lt;100,$D$75*A63*J63,$D$75*A63*K63))</f>
-        <v>10.98</v>
+        <f>IF($D$76*A63&lt;10,$D$76*A63*I63,IF($D$76*A63&lt;100,$D$76*A63*J63,$D$76*A63*K63))</f>
+        <v>10.470000000000001</v>
       </c>
     </row>
     <row r="64" spans="1:256">
       <c r="A64">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>U8</t>
+          <t>U6,U7,U11</t>
         </is>
       </c>
       <c r="C64" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Monolithic buck DC-DC</t>
-        </is>
-      </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
+          <t>2.85V low noise LDO</t>
+        </is>
+      </c>
+      <c r="E64" t="s">
+        <v>22</v>
       </c>
       <c r="F64" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>LMZ12001TZ-ADJ/NOPBCT-ND</t>
+          <t>MAX8510EXK29+TCT-ND</t>
         </is>
       </c>
       <c r="I64">
-        <v>7.9199999999999999</v>
+        <v>1.22</v>
       </c>
       <c r="J64">
-        <v>7.7000000000000002</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="K64">
-        <v>7.0499999999999998</v>
+        <v>0.80300000000000005</v>
       </c>
       <c r="M64">
-        <f>IF($D$75*A64&lt;10,$D$75*A64*I64,IF($D$75*A64&lt;100,$D$75*A64*J64,$D$75*A64*K64))</f>
-        <v>23.759999999999998</v>
+        <f>IF($D$76*A64&lt;10,$D$76*A64*I64,IF($D$76*A64&lt;100,$D$76*A64*J64,$D$76*A64*K64))</f>
+        <v>10.98</v>
       </c>
     </row>
     <row r="65" spans="1:256">
@@ -5050,49 +5053,42 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>U9</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>VENUS638FLPX-L</t>
-        </is>
+          <t>U8</t>
+        </is>
+      </c>
+      <c r="C65" t="s">
+        <v>27</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Single chip GPS COTS receiver</t>
+          <t>Monolithic buck DC-DC</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>SkyTraq</t>
-        </is>
-      </c>
-      <c r="F65" t="inlineStr">
-        <is>
-          <t>Venus638FLPx-L </t>
-        </is>
-      </c>
-      <c r="G65" t="s">
-        <v>9</v>
-      </c>
-      <c r="H65" t="inlineStr">
-        <is>
-          <t>Sparkfun GPS-10919</t>
+          <t>TI</t>
+        </is>
+      </c>
+      <c r="F65" t="s">
+        <v>27</v>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>LMZ12001TZ-ADJ/NOPBCT-ND</t>
         </is>
       </c>
       <c r="I65">
-        <v>39.950000000000003</v>
+        <v>7.9199999999999999</v>
       </c>
       <c r="J65">
-        <v>35.960000000000001</v>
+        <v>7.7000000000000002</v>
       </c>
       <c r="K65">
-        <v>31.960000000000001</v>
+        <v>7.0499999999999998</v>
       </c>
       <c r="M65">
-        <f>IF($D$75*A65&lt;10,$D$75*A65*I65,IF($D$75*A65&lt;100,$D$75*A65*J65,$D$75*A65*K65))</f>
-        <v>119.85000000000001</v>
+        <f>IF($D$76*A65&lt;10,$D$76*A65*I65,IF($D$76*A65&lt;100,$D$76*A65*J65,$D$76*A65*K65))</f>
+        <v>23.759999999999998</v>
       </c>
     </row>
     <row r="66" spans="1:256">
@@ -5101,45 +5097,49 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>U10</t>
-        </is>
-      </c>
-      <c r="C66" t="s">
-        <v>28</v>
+          <t>U9</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>VENUS838FLPX-L</t>
+        </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>L band splitter</t>
+          <t>Single chip GPS COTS receiver</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Minicircuits</t>
-        </is>
-      </c>
-      <c r="F66" t="s">
-        <v>28</v>
+          <t>SkyTraq</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>Venus838FLPx-L</t>
+        </is>
       </c>
       <c r="G66" t="s">
         <v>9</v>
       </c>
-      <c r="H66" s="10" t="inlineStr">
-        <is>
-          <t>MiniCircuits BP2G+</t>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>Tindie's Smokingresistor </t>
         </is>
       </c>
       <c r="I66">
-        <v>0.95999999999999996</v>
+        <v>39.950000000000003</v>
       </c>
       <c r="J66">
-        <v>0.95999999999999996</v>
+        <v>35.960000000000001</v>
       </c>
       <c r="K66">
-        <v>0.95999999999999996</v>
+        <v>31.960000000000001</v>
       </c>
       <c r="M66">
-        <f>IF($D$75*A66&lt;10,$D$75*A66*I66,IF($D$75*A66&lt;100,$D$75*A66*J66,$D$75*A66*K66))</f>
-        <v>2.8799999999999999</v>
+        <f>IF($D$76*A66&lt;10,$D$76*A66*I66,IF($D$76*A66&lt;100,$D$76*A66*J66,$D$76*A66*K66))</f>
+        <v>119.85000000000001</v>
       </c>
     </row>
     <row r="67" spans="1:256">
@@ -5148,49 +5148,45 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>U12</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>ALM-GP003</t>
-        </is>
+          <t>U10</t>
+        </is>
+      </c>
+      <c r="C67" t="s">
+        <v>28</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>L band SAW filter + LNA</t>
+          <t>L band splitter</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Avago</t>
-        </is>
-      </c>
-      <c r="F67" t="inlineStr">
-        <is>
-          <t>ALM-GP003-BLKG</t>
-        </is>
+          <t>Minicircuits</t>
+        </is>
+      </c>
+      <c r="F67" t="s">
+        <v>28</v>
       </c>
       <c r="G67" t="s">
         <v>9</v>
       </c>
       <c r="H67" s="10" t="inlineStr">
         <is>
-          <t>Mouser 630-ALM-GP003-BLKG</t>
+          <t>MiniCircuits BP2G+</t>
         </is>
       </c>
       <c r="I67">
-        <v>3.5899999999999999</v>
+        <v>0.95999999999999996</v>
       </c>
       <c r="J67">
+        <v>0.95999999999999996</v>
+      </c>
+      <c r="K67">
+        <v>0.95999999999999996</v>
+      </c>
+      <c r="M67">
+        <f>IF($D$76*A67&lt;10,$D$76*A67*I67,IF($D$76*A67&lt;100,$D$76*A67*J67,$D$76*A67*K67))</f>
         <v>2.8799999999999999</v>
-      </c>
-      <c r="K67">
-        <v>2.4399999999999999</v>
-      </c>
-      <c r="M67">
-        <f>IF($D$75*A67&lt;10,$D$75*A67*I67,IF($D$75*A67&lt;100,$D$75*A67*J67,$D$75*A67*K67))</f>
-        <v>10.77</v>
       </c>
     </row>
     <row r="68" spans="1:256">
@@ -5199,46 +5195,49 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>U13</t>
+          <t>U12</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>XC2C32A_VQ44_2</t>
+          <t>ALM-GP003</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>CPLD</t>
+          <t>L band SAW filter + LNA</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Xilinx</t>
+          <t>Avago</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>XC2C32A-6VQG44C</t>
-        </is>
-      </c>
-      <c r="G68" t="inlineStr">
-        <is>
-          <t>122-1404-ND</t>
+          <t>ALM-GP003-BLKG</t>
+        </is>
+      </c>
+      <c r="G68" t="s">
+        <v>9</v>
+      </c>
+      <c r="H68" s="10" t="inlineStr">
+        <is>
+          <t>Mouser 630-ALM-GP003-BLKG</t>
         </is>
       </c>
       <c r="I68">
-        <v>1.25</v>
+        <v>3.5899999999999999</v>
       </c>
       <c r="J68">
-        <v>1.25</v>
+        <v>2.8799999999999999</v>
       </c>
       <c r="K68">
-        <v>1.25</v>
+        <v>2.4399999999999999</v>
       </c>
       <c r="M68">
-        <f>IF($D$75*A68&lt;10,$D$75*A68*I68,IF($D$75*A68&lt;100,$D$75*A68*J68,$D$75*A68*K68))</f>
-        <v>3.75</v>
+        <f>IF($D$76*A68&lt;10,$D$76*A68*I68,IF($D$76*A68&lt;100,$D$76*A68*J68,$D$76*A68*K68))</f>
+        <v>10.77</v>
       </c>
     </row>
     <row r="69" spans="1:256">
@@ -5247,7 +5246,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>U14</t>
+          <t>U13</t>
         </is>
       </c>
       <c r="C69" t="s">
@@ -5255,366 +5254,404 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>1.8V LDO</t>
-        </is>
-      </c>
-      <c r="E69" t="s">
-        <v>23</v>
+          <t>CPLD</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Xilinx</t>
+        </is>
       </c>
       <c r="F69" t="s">
         <v>29</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
+          <t>122-1420-ND</t>
+        </is>
+      </c>
+      <c r="I69">
+        <v>1.25</v>
+      </c>
+      <c r="J69">
+        <v>1.25</v>
+      </c>
+      <c r="K69">
+        <v>1.25</v>
+      </c>
+      <c r="M69">
+        <f>IF($D$76*A69&lt;10,$D$76*A69*I69,IF($D$76*A69&lt;100,$D$76*A69*J69,$D$76*A69*K69))</f>
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="70" spans="1:256">
+      <c r="A70">
+        <v>1</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>U14</t>
+        </is>
+      </c>
+      <c r="C70" t="s">
+        <v>30</v>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>1.8V LDO</t>
+        </is>
+      </c>
+      <c r="E70" t="s">
+        <v>23</v>
+      </c>
+      <c r="F70" t="s">
+        <v>30</v>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
           <t>576-2864-1-ND</t>
         </is>
       </c>
-      <c r="H69" s="10" t="s">
+      <c r="H70" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="I69">
+      <c r="I70">
         <v>2.71</v>
       </c>
-      <c r="J69">
+      <c r="J70">
         <v>2.4500000000000002</v>
       </c>
-      <c r="K69">
+      <c r="K70">
         <v>1.97</v>
       </c>
-      <c r="M69">
-        <f>IF($D$75*A69&lt;10,$D$75*A69*I69,IF($D$75*A69&lt;100,$D$75*A69*J69,$D$75*A69*K69))</f>
+      <c r="M70">
+        <f>IF($D$76*A70&lt;10,$D$76*A70*I70,IF($D$76*A70&lt;100,$D$76*A70*J70,$D$76*A70*K70))</f>
         <v>8.129999999999999</v>
       </c>
     </row>
-    <row r="70" spans="1:256">
-      <c r="A70" s="7"/>
-      <c r="B70" s="7"/>
-      <c r="C70" s="8"/>
-      <c r="D70" s="7"/>
-      <c r="E70" s="7"/>
-      <c r="F70" s="7"/>
-      <c r="G70" s="7"/>
-      <c r="H70" s="7"/>
-      <c r="I70" s="9"/>
-      <c r="J70" s="9"/>
-      <c r="K70" s="9"/>
-      <c r="L70" s="7"/>
-      <c r="M70" s="9"/>
-      <c r="N70" s="7"/>
-      <c r="O70" s="7"/>
-      <c r="P70" s="7"/>
-      <c r="Q70" s="7"/>
-      <c r="R70" s="7"/>
-      <c r="S70" s="7"/>
-      <c r="T70" s="7"/>
-      <c r="U70" s="7"/>
-      <c r="V70" s="7"/>
-      <c r="W70" s="7"/>
-      <c r="X70" s="7"/>
-      <c r="Y70" s="7"/>
-      <c r="Z70" s="7"/>
-      <c r="AA70" s="7"/>
-      <c r="AB70" s="7"/>
-      <c r="AC70" s="7"/>
-      <c r="AD70" s="7"/>
-      <c r="AE70" s="7"/>
-      <c r="AF70" s="7"/>
-      <c r="AG70" s="7"/>
-      <c r="AH70" s="7"/>
-      <c r="AI70" s="7"/>
-      <c r="AJ70" s="7"/>
-      <c r="AK70" s="7"/>
-      <c r="AL70" s="7"/>
-      <c r="AM70" s="7"/>
-      <c r="AN70" s="7"/>
-      <c r="AO70" s="7"/>
-      <c r="AP70" s="7"/>
-      <c r="AQ70" s="7"/>
-      <c r="AR70" s="7"/>
-      <c r="AS70" s="7"/>
-      <c r="AT70" s="7"/>
-      <c r="AU70" s="7"/>
-      <c r="AV70" s="7"/>
-      <c r="AW70" s="7"/>
-      <c r="AX70" s="7"/>
-      <c r="AY70" s="7"/>
-      <c r="AZ70" s="7"/>
-      <c r="BA70" s="7"/>
-      <c r="BB70" s="7"/>
-      <c r="BC70" s="7"/>
-      <c r="BD70" s="7"/>
-      <c r="BE70" s="7"/>
-      <c r="BF70" s="7"/>
-      <c r="BG70" s="7"/>
-      <c r="BH70" s="7"/>
-      <c r="BI70" s="7"/>
-      <c r="BJ70" s="7"/>
-      <c r="BK70" s="7"/>
-      <c r="BL70" s="7"/>
-      <c r="BM70" s="7"/>
-      <c r="BN70" s="7"/>
-      <c r="BO70" s="7"/>
-      <c r="BP70" s="7"/>
-      <c r="BQ70" s="7"/>
-      <c r="BR70" s="7"/>
-      <c r="BS70" s="7"/>
-      <c r="BT70" s="7"/>
-      <c r="BU70" s="7"/>
-      <c r="BV70" s="7"/>
-      <c r="BW70" s="7"/>
-      <c r="BX70" s="7"/>
-      <c r="BY70" s="7"/>
-      <c r="BZ70" s="7"/>
-      <c r="CA70" s="7"/>
-      <c r="CB70" s="7"/>
-      <c r="CC70" s="7"/>
-      <c r="CD70" s="7"/>
-      <c r="CE70" s="7"/>
-      <c r="CF70" s="7"/>
-      <c r="CG70" s="7"/>
-      <c r="CH70" s="7"/>
-      <c r="CI70" s="7"/>
-      <c r="CJ70" s="7"/>
-      <c r="CK70" s="7"/>
-      <c r="CL70" s="7"/>
-      <c r="CM70" s="7"/>
-      <c r="CN70" s="7"/>
-      <c r="CO70" s="7"/>
-      <c r="CP70" s="7"/>
-      <c r="CQ70" s="7"/>
-      <c r="CR70" s="7"/>
-      <c r="CS70" s="7"/>
-      <c r="CT70" s="7"/>
-      <c r="CU70" s="7"/>
-      <c r="CV70" s="7"/>
-      <c r="CW70" s="7"/>
-      <c r="CX70" s="7"/>
-      <c r="CY70" s="7"/>
-      <c r="CZ70" s="7"/>
-      <c r="DA70" s="7"/>
-      <c r="DB70" s="7"/>
-      <c r="DC70" s="7"/>
-      <c r="DD70" s="7"/>
-      <c r="DE70" s="7"/>
-      <c r="DF70" s="7"/>
-      <c r="DG70" s="7"/>
-      <c r="DH70" s="7"/>
-      <c r="DI70" s="7"/>
-      <c r="DJ70" s="7"/>
-      <c r="DK70" s="7"/>
-      <c r="DL70" s="7"/>
-      <c r="DM70" s="7"/>
-      <c r="DN70" s="7"/>
-      <c r="DO70" s="7"/>
-      <c r="DP70" s="7"/>
-      <c r="DQ70" s="7"/>
-      <c r="DR70" s="7"/>
-      <c r="DS70" s="7"/>
-      <c r="DT70" s="7"/>
-      <c r="DU70" s="7"/>
-      <c r="DV70" s="7"/>
-      <c r="DW70" s="7"/>
-      <c r="DX70" s="7"/>
-      <c r="DY70" s="7"/>
-      <c r="DZ70" s="7"/>
-      <c r="EA70" s="7"/>
-      <c r="EB70" s="7"/>
-      <c r="EC70" s="7"/>
-      <c r="ED70" s="7"/>
-      <c r="EE70" s="7"/>
-      <c r="EF70" s="7"/>
-      <c r="EG70" s="7"/>
-      <c r="EH70" s="7"/>
-      <c r="EI70" s="7"/>
-      <c r="EJ70" s="7"/>
-      <c r="EK70" s="7"/>
-      <c r="EL70" s="7"/>
-      <c r="EM70" s="7"/>
-      <c r="EN70" s="7"/>
-      <c r="EO70" s="7"/>
-      <c r="EP70" s="7"/>
-      <c r="EQ70" s="7"/>
-      <c r="ER70" s="7"/>
-      <c r="ES70" s="7"/>
-      <c r="ET70" s="7"/>
-      <c r="EU70" s="7"/>
-      <c r="EV70" s="7"/>
-      <c r="EW70" s="7"/>
-      <c r="EX70" s="7"/>
-      <c r="EY70" s="7"/>
-      <c r="EZ70" s="7"/>
-      <c r="FA70" s="7"/>
-      <c r="FB70" s="7"/>
-      <c r="FC70" s="7"/>
-      <c r="FD70" s="7"/>
-      <c r="FE70" s="7"/>
-      <c r="FF70" s="7"/>
-      <c r="FG70" s="7"/>
-      <c r="FH70" s="7"/>
-      <c r="FI70" s="7"/>
-      <c r="FJ70" s="7"/>
-      <c r="FK70" s="7"/>
-      <c r="FL70" s="7"/>
-      <c r="FM70" s="7"/>
-      <c r="FN70" s="7"/>
-      <c r="FO70" s="7"/>
-      <c r="FP70" s="7"/>
-      <c r="FQ70" s="7"/>
-      <c r="FR70" s="7"/>
-      <c r="FS70" s="7"/>
-      <c r="FT70" s="7"/>
-      <c r="FU70" s="7"/>
-      <c r="FV70" s="7"/>
-      <c r="FW70" s="7"/>
-      <c r="FX70" s="7"/>
-      <c r="FY70" s="7"/>
-      <c r="FZ70" s="7"/>
-      <c r="GA70" s="7"/>
-      <c r="GB70" s="7"/>
-      <c r="GC70" s="7"/>
-      <c r="GD70" s="7"/>
-      <c r="GE70" s="7"/>
-      <c r="GF70" s="7"/>
-      <c r="GG70" s="7"/>
-      <c r="GH70" s="7"/>
-      <c r="GI70" s="7"/>
-      <c r="GJ70" s="7"/>
-      <c r="GK70" s="7"/>
-      <c r="GL70" s="7"/>
-      <c r="GM70" s="7"/>
-      <c r="GN70" s="7"/>
-      <c r="GO70" s="7"/>
-      <c r="GP70" s="7"/>
-      <c r="GQ70" s="7"/>
-      <c r="GR70" s="7"/>
-      <c r="GS70" s="7"/>
-      <c r="GT70" s="7"/>
-      <c r="GU70" s="7"/>
-      <c r="GV70" s="7"/>
-      <c r="GW70" s="7"/>
-      <c r="GX70" s="7"/>
-      <c r="GY70" s="7"/>
-      <c r="GZ70" s="7"/>
-      <c r="HA70" s="7"/>
-      <c r="HB70" s="7"/>
-      <c r="HC70" s="7"/>
-      <c r="HD70" s="7"/>
-      <c r="HE70" s="7"/>
-      <c r="HF70" s="7"/>
-      <c r="HG70" s="7"/>
-      <c r="HH70" s="7"/>
-      <c r="HI70" s="7"/>
-      <c r="HJ70" s="7"/>
-      <c r="HK70" s="7"/>
-      <c r="HL70" s="7"/>
-      <c r="HM70" s="7"/>
-      <c r="HN70" s="7"/>
-      <c r="HO70" s="7"/>
-      <c r="HP70" s="7"/>
-      <c r="HQ70" s="7"/>
-      <c r="HR70" s="7"/>
-      <c r="HS70" s="7"/>
-      <c r="HT70" s="7"/>
-      <c r="HU70" s="7"/>
-      <c r="HV70" s="7"/>
-      <c r="HW70" s="7"/>
-      <c r="HX70" s="7"/>
-      <c r="HY70" s="7"/>
-      <c r="HZ70" s="7"/>
-      <c r="IA70" s="7"/>
-      <c r="IB70" s="7"/>
-      <c r="IC70" s="7"/>
-      <c r="ID70" s="7"/>
-      <c r="IE70" s="7"/>
-      <c r="IF70" s="7"/>
-      <c r="IG70" s="7"/>
-      <c r="IH70" s="7"/>
-      <c r="II70" s="7"/>
-      <c r="IJ70" s="7"/>
-      <c r="IK70" s="7"/>
-      <c r="IL70" s="7"/>
-      <c r="IM70" s="7"/>
-      <c r="IN70" s="7"/>
-      <c r="IO70" s="7"/>
-      <c r="IP70" s="7"/>
-      <c r="IQ70" s="7"/>
-      <c r="IR70" s="7"/>
-      <c r="IS70" s="7"/>
-      <c r="IT70" s="7"/>
-      <c r="IU70" s="7"/>
-    </row>
     <row r="71" spans="1:256">
-      <c r="A71">
+      <c r="A71" s="7"/>
+      <c r="B71" s="7"/>
+      <c r="C71" s="8"/>
+      <c r="D71" s="7"/>
+      <c r="E71" s="7"/>
+      <c r="F71" s="7"/>
+      <c r="G71" s="7"/>
+      <c r="H71" s="7"/>
+      <c r="I71" s="9"/>
+      <c r="J71" s="9"/>
+      <c r="K71" s="9"/>
+      <c r="L71" s="7"/>
+      <c r="M71" s="9"/>
+      <c r="N71" s="7"/>
+      <c r="O71" s="7"/>
+      <c r="P71" s="7"/>
+      <c r="Q71" s="7"/>
+      <c r="R71" s="7"/>
+      <c r="S71" s="7"/>
+      <c r="T71" s="7"/>
+      <c r="U71" s="7"/>
+      <c r="V71" s="7"/>
+      <c r="W71" s="7"/>
+      <c r="X71" s="7"/>
+      <c r="Y71" s="7"/>
+      <c r="Z71" s="7"/>
+      <c r="AA71" s="7"/>
+      <c r="AB71" s="7"/>
+      <c r="AC71" s="7"/>
+      <c r="AD71" s="7"/>
+      <c r="AE71" s="7"/>
+      <c r="AF71" s="7"/>
+      <c r="AG71" s="7"/>
+      <c r="AH71" s="7"/>
+      <c r="AI71" s="7"/>
+      <c r="AJ71" s="7"/>
+      <c r="AK71" s="7"/>
+      <c r="AL71" s="7"/>
+      <c r="AM71" s="7"/>
+      <c r="AN71" s="7"/>
+      <c r="AO71" s="7"/>
+      <c r="AP71" s="7"/>
+      <c r="AQ71" s="7"/>
+      <c r="AR71" s="7"/>
+      <c r="AS71" s="7"/>
+      <c r="AT71" s="7"/>
+      <c r="AU71" s="7"/>
+      <c r="AV71" s="7"/>
+      <c r="AW71" s="7"/>
+      <c r="AX71" s="7"/>
+      <c r="AY71" s="7"/>
+      <c r="AZ71" s="7"/>
+      <c r="BA71" s="7"/>
+      <c r="BB71" s="7"/>
+      <c r="BC71" s="7"/>
+      <c r="BD71" s="7"/>
+      <c r="BE71" s="7"/>
+      <c r="BF71" s="7"/>
+      <c r="BG71" s="7"/>
+      <c r="BH71" s="7"/>
+      <c r="BI71" s="7"/>
+      <c r="BJ71" s="7"/>
+      <c r="BK71" s="7"/>
+      <c r="BL71" s="7"/>
+      <c r="BM71" s="7"/>
+      <c r="BN71" s="7"/>
+      <c r="BO71" s="7"/>
+      <c r="BP71" s="7"/>
+      <c r="BQ71" s="7"/>
+      <c r="BR71" s="7"/>
+      <c r="BS71" s="7"/>
+      <c r="BT71" s="7"/>
+      <c r="BU71" s="7"/>
+      <c r="BV71" s="7"/>
+      <c r="BW71" s="7"/>
+      <c r="BX71" s="7"/>
+      <c r="BY71" s="7"/>
+      <c r="BZ71" s="7"/>
+      <c r="CA71" s="7"/>
+      <c r="CB71" s="7"/>
+      <c r="CC71" s="7"/>
+      <c r="CD71" s="7"/>
+      <c r="CE71" s="7"/>
+      <c r="CF71" s="7"/>
+      <c r="CG71" s="7"/>
+      <c r="CH71" s="7"/>
+      <c r="CI71" s="7"/>
+      <c r="CJ71" s="7"/>
+      <c r="CK71" s="7"/>
+      <c r="CL71" s="7"/>
+      <c r="CM71" s="7"/>
+      <c r="CN71" s="7"/>
+      <c r="CO71" s="7"/>
+      <c r="CP71" s="7"/>
+      <c r="CQ71" s="7"/>
+      <c r="CR71" s="7"/>
+      <c r="CS71" s="7"/>
+      <c r="CT71" s="7"/>
+      <c r="CU71" s="7"/>
+      <c r="CV71" s="7"/>
+      <c r="CW71" s="7"/>
+      <c r="CX71" s="7"/>
+      <c r="CY71" s="7"/>
+      <c r="CZ71" s="7"/>
+      <c r="DA71" s="7"/>
+      <c r="DB71" s="7"/>
+      <c r="DC71" s="7"/>
+      <c r="DD71" s="7"/>
+      <c r="DE71" s="7"/>
+      <c r="DF71" s="7"/>
+      <c r="DG71" s="7"/>
+      <c r="DH71" s="7"/>
+      <c r="DI71" s="7"/>
+      <c r="DJ71" s="7"/>
+      <c r="DK71" s="7"/>
+      <c r="DL71" s="7"/>
+      <c r="DM71" s="7"/>
+      <c r="DN71" s="7"/>
+      <c r="DO71" s="7"/>
+      <c r="DP71" s="7"/>
+      <c r="DQ71" s="7"/>
+      <c r="DR71" s="7"/>
+      <c r="DS71" s="7"/>
+      <c r="DT71" s="7"/>
+      <c r="DU71" s="7"/>
+      <c r="DV71" s="7"/>
+      <c r="DW71" s="7"/>
+      <c r="DX71" s="7"/>
+      <c r="DY71" s="7"/>
+      <c r="DZ71" s="7"/>
+      <c r="EA71" s="7"/>
+      <c r="EB71" s="7"/>
+      <c r="EC71" s="7"/>
+      <c r="ED71" s="7"/>
+      <c r="EE71" s="7"/>
+      <c r="EF71" s="7"/>
+      <c r="EG71" s="7"/>
+      <c r="EH71" s="7"/>
+      <c r="EI71" s="7"/>
+      <c r="EJ71" s="7"/>
+      <c r="EK71" s="7"/>
+      <c r="EL71" s="7"/>
+      <c r="EM71" s="7"/>
+      <c r="EN71" s="7"/>
+      <c r="EO71" s="7"/>
+      <c r="EP71" s="7"/>
+      <c r="EQ71" s="7"/>
+      <c r="ER71" s="7"/>
+      <c r="ES71" s="7"/>
+      <c r="ET71" s="7"/>
+      <c r="EU71" s="7"/>
+      <c r="EV71" s="7"/>
+      <c r="EW71" s="7"/>
+      <c r="EX71" s="7"/>
+      <c r="EY71" s="7"/>
+      <c r="EZ71" s="7"/>
+      <c r="FA71" s="7"/>
+      <c r="FB71" s="7"/>
+      <c r="FC71" s="7"/>
+      <c r="FD71" s="7"/>
+      <c r="FE71" s="7"/>
+      <c r="FF71" s="7"/>
+      <c r="FG71" s="7"/>
+      <c r="FH71" s="7"/>
+      <c r="FI71" s="7"/>
+      <c r="FJ71" s="7"/>
+      <c r="FK71" s="7"/>
+      <c r="FL71" s="7"/>
+      <c r="FM71" s="7"/>
+      <c r="FN71" s="7"/>
+      <c r="FO71" s="7"/>
+      <c r="FP71" s="7"/>
+      <c r="FQ71" s="7"/>
+      <c r="FR71" s="7"/>
+      <c r="FS71" s="7"/>
+      <c r="FT71" s="7"/>
+      <c r="FU71" s="7"/>
+      <c r="FV71" s="7"/>
+      <c r="FW71" s="7"/>
+      <c r="FX71" s="7"/>
+      <c r="FY71" s="7"/>
+      <c r="FZ71" s="7"/>
+      <c r="GA71" s="7"/>
+      <c r="GB71" s="7"/>
+      <c r="GC71" s="7"/>
+      <c r="GD71" s="7"/>
+      <c r="GE71" s="7"/>
+      <c r="GF71" s="7"/>
+      <c r="GG71" s="7"/>
+      <c r="GH71" s="7"/>
+      <c r="GI71" s="7"/>
+      <c r="GJ71" s="7"/>
+      <c r="GK71" s="7"/>
+      <c r="GL71" s="7"/>
+      <c r="GM71" s="7"/>
+      <c r="GN71" s="7"/>
+      <c r="GO71" s="7"/>
+      <c r="GP71" s="7"/>
+      <c r="GQ71" s="7"/>
+      <c r="GR71" s="7"/>
+      <c r="GS71" s="7"/>
+      <c r="GT71" s="7"/>
+      <c r="GU71" s="7"/>
+      <c r="GV71" s="7"/>
+      <c r="GW71" s="7"/>
+      <c r="GX71" s="7"/>
+      <c r="GY71" s="7"/>
+      <c r="GZ71" s="7"/>
+      <c r="HA71" s="7"/>
+      <c r="HB71" s="7"/>
+      <c r="HC71" s="7"/>
+      <c r="HD71" s="7"/>
+      <c r="HE71" s="7"/>
+      <c r="HF71" s="7"/>
+      <c r="HG71" s="7"/>
+      <c r="HH71" s="7"/>
+      <c r="HI71" s="7"/>
+      <c r="HJ71" s="7"/>
+      <c r="HK71" s="7"/>
+      <c r="HL71" s="7"/>
+      <c r="HM71" s="7"/>
+      <c r="HN71" s="7"/>
+      <c r="HO71" s="7"/>
+      <c r="HP71" s="7"/>
+      <c r="HQ71" s="7"/>
+      <c r="HR71" s="7"/>
+      <c r="HS71" s="7"/>
+      <c r="HT71" s="7"/>
+      <c r="HU71" s="7"/>
+      <c r="HV71" s="7"/>
+      <c r="HW71" s="7"/>
+      <c r="HX71" s="7"/>
+      <c r="HY71" s="7"/>
+      <c r="HZ71" s="7"/>
+      <c r="IA71" s="7"/>
+      <c r="IB71" s="7"/>
+      <c r="IC71" s="7"/>
+      <c r="ID71" s="7"/>
+      <c r="IE71" s="7"/>
+      <c r="IF71" s="7"/>
+      <c r="IG71" s="7"/>
+      <c r="IH71" s="7"/>
+      <c r="II71" s="7"/>
+      <c r="IJ71" s="7"/>
+      <c r="IK71" s="7"/>
+      <c r="IL71" s="7"/>
+      <c r="IM71" s="7"/>
+      <c r="IN71" s="7"/>
+      <c r="IO71" s="7"/>
+      <c r="IP71" s="7"/>
+      <c r="IQ71" s="7"/>
+      <c r="IR71" s="7"/>
+      <c r="IS71" s="7"/>
+      <c r="IT71" s="7"/>
+      <c r="IU71" s="7"/>
+    </row>
+    <row r="72" spans="1:256">
+      <c r="A72">
         <v>1</v>
       </c>
-      <c r="B71" t="inlineStr">
+      <c r="B72" t="inlineStr">
         <is>
           <t>X1</t>
         </is>
       </c>
-      <c r="C71" t="inlineStr">
+      <c r="C72" t="inlineStr">
         <is>
           <t>25 MHz</t>
         </is>
       </c>
-      <c r="D71" t="inlineStr">
+      <c r="D72" t="inlineStr">
         <is>
           <t>25 Mhz SMT crystal, 20ppm</t>
         </is>
       </c>
-      <c r="E71" t="s">
+      <c r="E72" t="s">
         <v>25</v>
       </c>
-      <c r="F71" t="inlineStr">
+      <c r="F72" t="inlineStr">
         <is>
           <t>8Y-25.000MEEQ-T</t>
         </is>
       </c>
-      <c r="G71" t="inlineStr">
+      <c r="G72" t="inlineStr">
         <is>
           <t>887-1819-1-ND</t>
         </is>
       </c>
-      <c r="I71">
+      <c r="I72">
         <v>1.8899999999999999</v>
       </c>
-      <c r="J71">
+      <c r="J72">
         <v>1.8100000000000001</v>
       </c>
-      <c r="K71">
+      <c r="K72">
         <v>1.512</v>
       </c>
-      <c r="M71">
-        <f>IF($D$75*A71&lt;10,$D$75*A71*I71,IF($D$75*A71&lt;100,$D$75*A71*J71,$D$75*A71*K71))</f>
+      <c r="M72">
+        <f>IF($D$76*A72&lt;10,$D$76*A72*I72,IF($D$76*A72&lt;100,$D$76*A72*J72,$D$76*A72*K72))</f>
         <v>5.6699999999999999</v>
       </c>
     </row>
-    <row r="73" spans="1:256">
-      <c r="L73" s="3" t="inlineStr">
+    <row r="74" spans="1:256">
+      <c r="L74" s="3" t="inlineStr">
         <is>
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="M73" s="15">
-        <f>SUM(M2:M71)</f>
-        <v>397.32749999999999</v>
-      </c>
-    </row>
-    <row r="75" spans="1:256">
-      <c r="A75" s="3" t="inlineStr">
+      <c r="M74" s="15">
+        <f>SUM(M2:M72)</f>
+        <v>397.6275</v>
+      </c>
+    </row>
+    <row r="76" spans="1:256">
+      <c r="A76" s="3" t="inlineStr">
         <is>
           <t>Boards to manufacture: </t>
         </is>
       </c>
-      <c r="D75" s="3">
+      <c r="D76" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="65524" spans="1:256">
-      <c r="C65524" s="0"/>
-      <c r="I65524" s="0"/>
-      <c r="J65524" s="0"/>
-      <c r="K65524" s="0"/>
     </row>
     <row r="65525" spans="1:256">
       <c r="C65525" s="0"/>
@@ -5688,11 +5725,11 @@
       <c r="J65536" s="0"/>
       <c r="K65536" s="0"/>
     </row>
-    <row r="1048571" spans="1:256">
-      <c r="C1048571" s="0"/>
-      <c r="I1048571" s="0"/>
-      <c r="J1048571" s="0"/>
-      <c r="K1048571" s="0"/>
+    <row r="65537" spans="1:256">
+      <c r="C65537" s="0"/>
+      <c r="I65537" s="0"/>
+      <c r="J65537" s="0"/>
+      <c r="K65537" s="0"/>
     </row>
     <row r="1048572" spans="1:256">
       <c r="C1048572" s="0"/>

</xml_diff>